<commit_message>
relocating files of deprecated phenotypes
</commit_message>
<xml_diff>
--- a/extras/PhenotypeDescription.xlsx
+++ b/extras/PhenotypeDescription.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\github\ohdsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\github\ohdsi\PhenotypeLibrary\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2532,8 +2532,8 @@
   <dimension ref="A1:I266"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6252,7 +6252,7 @@
         <v>441848000</v>
       </c>
       <c r="B175">
-        <v>441848000</v>
+        <v>0</v>
       </c>
       <c r="C175">
         <v>441848000</v>
@@ -8213,7 +8213,7 @@
         <v>46271022000</v>
       </c>
       <c r="B266">
-        <v>46271022000</v>
+        <v>4030518000</v>
       </c>
       <c r="C266">
         <v>46271022000</v>

</xml_diff>

<commit_message>
add inflammatory disease of mediastinum
</commit_message>
<xml_diff>
--- a/extras/PhenotypeDescription.xlsx
+++ b/extras/PhenotypeDescription.xlsx
@@ -2561,9 +2561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7681,93 +7681,93 @@
         <v>287</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A235">
+        <v>4195694000</v>
+      </c>
+      <c r="B235">
+        <v>4195694000</v>
+      </c>
+      <c r="C235">
+        <v>4195694000</v>
+      </c>
+      <c r="D235" t="s">
+        <v>405</v>
+      </c>
+      <c r="E235">
+        <v>4195694</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H235" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A236">
         <v>4201096000</v>
       </c>
-      <c r="B235">
+      <c r="B236">
         <v>4190307000</v>
       </c>
-      <c r="C235">
+      <c r="C236">
         <v>4201096000</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D236" t="s">
         <v>408</v>
       </c>
-      <c r="E235">
+      <c r="E236">
         <v>4201096</v>
       </c>
-      <c r="F235" s="1" t="s">
+      <c r="F236" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="I235" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="236" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A236">
-        <v>4195694000</v>
-      </c>
-      <c r="B236">
-        <v>4195694000</v>
-      </c>
-      <c r="C236">
-        <v>4195694000</v>
-      </c>
-      <c r="D236" t="s">
-        <v>405</v>
-      </c>
-      <c r="E236">
-        <v>4195694</v>
-      </c>
-      <c r="F236" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="H236" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="237" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="I236" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A237">
+        <v>4212540000</v>
+      </c>
+      <c r="B237">
+        <v>4212540000</v>
+      </c>
+      <c r="C237">
+        <v>4212540000</v>
+      </c>
+      <c r="D237" t="s">
+        <v>410</v>
+      </c>
+      <c r="E237">
+        <v>4212540</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A238">
         <v>4223659000</v>
       </c>
-      <c r="B237">
+      <c r="B238">
         <v>4094294000</v>
       </c>
-      <c r="C237">
+      <c r="C238">
         <v>4223659000</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D238" t="s">
         <v>412</v>
       </c>
-      <c r="E237">
+      <c r="E238">
         <v>4223659</v>
       </c>
-      <c r="F237" s="1" t="s">
+      <c r="F238" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="I237" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9" ht="240" x14ac:dyDescent="0.25">
-      <c r="A238">
-        <v>4212540000</v>
-      </c>
-      <c r="B238">
-        <v>4212540000</v>
-      </c>
-      <c r="C238">
-        <v>4212540000</v>
-      </c>
-      <c r="D238" t="s">
-        <v>410</v>
-      </c>
-      <c r="E238">
-        <v>4212540</v>
-      </c>
-      <c r="F238" s="1" t="s">
-        <v>411</v>
+      <c r="I238" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="239" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -7810,208 +7810,208 @@
         <v>416</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A241">
+        <v>4246127000</v>
+      </c>
+      <c r="B241">
+        <v>4246127000</v>
+      </c>
+      <c r="C241">
+        <v>4246127000</v>
+      </c>
+      <c r="D241" t="s">
+        <v>417</v>
+      </c>
+      <c r="E241">
+        <v>4246127</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="H241" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A242">
         <v>4253901000</v>
       </c>
-      <c r="B241">
+      <c r="B242">
         <v>73553000</v>
       </c>
-      <c r="C241">
+      <c r="C242">
         <v>4253901000</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D242" t="s">
         <v>419</v>
       </c>
-      <c r="E241">
+      <c r="E242">
         <v>4253901</v>
       </c>
-      <c r="F241" s="1" t="s">
+      <c r="F242" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="I241" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="242" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A242">
-        <v>4246127000</v>
-      </c>
-      <c r="B242">
-        <v>4246127000</v>
-      </c>
-      <c r="C242">
-        <v>4246127000</v>
-      </c>
-      <c r="D242" t="s">
-        <v>417</v>
-      </c>
-      <c r="E242">
-        <v>4246127</v>
-      </c>
-      <c r="F242" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="H242" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="243" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="I242" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A243">
+        <v>4256228000</v>
+      </c>
+      <c r="B243">
+        <v>4256228000</v>
+      </c>
+      <c r="C243">
+        <v>4256228000</v>
+      </c>
+      <c r="D243" t="s">
+        <v>421</v>
+      </c>
+      <c r="E243">
+        <v>4256228</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="H243" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A244">
         <v>4260535000</v>
       </c>
-      <c r="B243">
+      <c r="B244">
         <v>4043371000</v>
       </c>
-      <c r="C243">
+      <c r="C244">
         <v>4260535000</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D244" t="s">
         <v>424</v>
       </c>
-      <c r="E243">
+      <c r="E244">
         <v>4260535</v>
       </c>
-      <c r="F243" s="1" t="s">
+      <c r="F244" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="H243" t="s">
+      <c r="H244" t="s">
         <v>425</v>
       </c>
-      <c r="I243" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="244" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A244">
-        <v>4256228000</v>
-      </c>
-      <c r="B244">
-        <v>4256228000</v>
-      </c>
-      <c r="C244">
-        <v>4256228000</v>
-      </c>
-      <c r="D244" t="s">
-        <v>421</v>
-      </c>
-      <c r="E244">
-        <v>4256228</v>
-      </c>
-      <c r="F244" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="H244" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="245" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I244" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A245">
+        <v>4266367000</v>
+      </c>
+      <c r="B245">
+        <v>4266367000</v>
+      </c>
+      <c r="C245">
+        <v>4266367000</v>
+      </c>
+      <c r="D245" t="s">
+        <v>426</v>
+      </c>
+      <c r="E245">
+        <v>4266367</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A246">
         <v>4272240000</v>
       </c>
-      <c r="B245">
+      <c r="B246">
         <v>4094294000</v>
       </c>
-      <c r="C245">
+      <c r="C246">
         <v>4272240000</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D246" t="s">
         <v>428</v>
       </c>
-      <c r="E245">
+      <c r="E246">
         <v>4272240</v>
       </c>
-      <c r="F245" s="1" t="s">
+      <c r="F246" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="I245" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="246" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A246">
-        <v>4266367000</v>
-      </c>
-      <c r="B246">
-        <v>4266367000</v>
-      </c>
-      <c r="C246">
-        <v>4266367000</v>
-      </c>
-      <c r="D246" t="s">
-        <v>426</v>
-      </c>
-      <c r="E246">
-        <v>4266367</v>
-      </c>
-      <c r="F246" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="247" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="I246" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A247">
+        <v>4273391000</v>
+      </c>
+      <c r="B247">
+        <v>4273391000</v>
+      </c>
+      <c r="C247">
+        <v>4273391000</v>
+      </c>
+      <c r="D247" t="s">
+        <v>429</v>
+      </c>
+      <c r="E247">
+        <v>4273391</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A248">
         <v>4281232000</v>
       </c>
-      <c r="B247">
+      <c r="B248">
         <v>4212540000</v>
       </c>
-      <c r="C247">
+      <c r="C248">
         <v>4281232000</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D248" t="s">
         <v>431</v>
       </c>
-      <c r="E247">
+      <c r="E248">
         <v>4281232</v>
       </c>
-      <c r="F247" s="1" t="s">
+      <c r="F248" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="I247" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="248" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A248">
+      <c r="I248" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A249">
         <v>4284492000</v>
       </c>
-      <c r="B248">
+      <c r="B249">
         <v>140168000</v>
       </c>
-      <c r="C248">
+      <c r="C249">
         <v>4284492000</v>
       </c>
-      <c r="D248" s="3" t="s">
+      <c r="D249" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="E248">
+      <c r="E249">
         <v>4284492</v>
       </c>
-      <c r="F248" s="1" t="s">
+      <c r="F249" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="I248" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="249" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A249">
-        <v>4273391000</v>
-      </c>
-      <c r="B249">
-        <v>4273391000</v>
-      </c>
-      <c r="C249">
-        <v>4273391000</v>
-      </c>
-      <c r="D249" t="s">
-        <v>429</v>
-      </c>
-      <c r="E249">
-        <v>4273391</v>
-      </c>
-      <c r="F249" s="1" t="s">
-        <v>430</v>
+      <c r="I249" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="250" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8036,45 +8036,45 @@
     </row>
     <row r="251" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>4290976000</v>
+        <v>4286201000</v>
       </c>
       <c r="B251">
-        <v>4137275000</v>
+        <v>4286201000</v>
       </c>
       <c r="C251">
-        <v>4290976000</v>
+        <v>4286201000</v>
       </c>
       <c r="D251" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E251">
-        <v>4290976</v>
+        <v>4286201</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="I251" t="s">
-        <v>22</v>
+        <v>437</v>
       </c>
     </row>
     <row r="252" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>4286201000</v>
+        <v>4290976000</v>
       </c>
       <c r="B252">
-        <v>4286201000</v>
+        <v>4137275000</v>
       </c>
       <c r="C252">
-        <v>4286201000</v>
+        <v>4290976000</v>
       </c>
       <c r="D252" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E252">
-        <v>4286201</v>
+        <v>4290976</v>
       </c>
       <c r="F252" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
+      </c>
+      <c r="I252" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="253" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8117,96 +8117,96 @@
         <v>443</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A255">
+        <v>4311499000</v>
+      </c>
+      <c r="B255">
+        <v>4311499000</v>
+      </c>
+      <c r="C255">
+        <v>4311499000</v>
+      </c>
+      <c r="D255" t="s">
+        <v>444</v>
+      </c>
+      <c r="E255">
+        <v>4311499</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H255" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A256">
         <v>4318985000</v>
       </c>
-      <c r="B255">
+      <c r="B256">
         <v>378416000</v>
       </c>
-      <c r="C255">
+      <c r="C256">
         <v>4318985000</v>
       </c>
-      <c r="D255" t="s">
+      <c r="D256" t="s">
         <v>446</v>
       </c>
-      <c r="E255">
+      <c r="E256">
         <v>4318985</v>
       </c>
-      <c r="F255" s="1" t="s">
+      <c r="F256" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="I255" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="256" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A256">
-        <v>4311499000</v>
-      </c>
-      <c r="B256">
-        <v>4311499000</v>
-      </c>
-      <c r="C256">
-        <v>4311499000</v>
-      </c>
-      <c r="D256" t="s">
-        <v>444</v>
-      </c>
-      <c r="E256">
-        <v>4311499</v>
-      </c>
-      <c r="F256" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="H256" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="257" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="I256" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A257">
+        <v>4322024000</v>
+      </c>
+      <c r="B257">
+        <v>4322024000</v>
+      </c>
+      <c r="C257">
+        <v>4322024000</v>
+      </c>
+      <c r="D257" t="s">
+        <v>447</v>
+      </c>
+      <c r="E257">
+        <v>4322024</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="H257" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A258">
         <v>4344489000</v>
       </c>
-      <c r="B257">
+      <c r="B258">
         <v>4137275000</v>
       </c>
-      <c r="C257">
+      <c r="C258">
         <v>4344489000</v>
       </c>
-      <c r="D257" t="s">
+      <c r="D258" t="s">
         <v>450</v>
       </c>
-      <c r="E257">
+      <c r="E258">
         <v>4344489</v>
       </c>
-      <c r="F257" s="1" t="s">
+      <c r="F258" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="I257" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="258" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A258">
-        <v>4322024000</v>
-      </c>
-      <c r="B258">
-        <v>4322024000</v>
-      </c>
-      <c r="C258">
-        <v>4322024000</v>
-      </c>
-      <c r="D258" t="s">
-        <v>447</v>
-      </c>
-      <c r="E258">
-        <v>4322024</v>
-      </c>
-      <c r="F258" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H258" t="s">
-        <v>449</v>
+      <c r="I258" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="259" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -8229,142 +8229,142 @@
         <v>452</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A260">
+        <v>37311061000</v>
+      </c>
+      <c r="B260">
+        <v>37311061000</v>
+      </c>
+      <c r="C260">
+        <v>37311061000</v>
+      </c>
+      <c r="D260" t="s">
+        <v>453</v>
+      </c>
+      <c r="E260">
+        <v>37311061</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A261">
         <v>40479589000</v>
       </c>
-      <c r="B260">
+      <c r="B261">
         <v>321319000</v>
       </c>
-      <c r="C260">
+      <c r="C261">
         <v>40479589000</v>
       </c>
-      <c r="D260" t="s">
+      <c r="D261" t="s">
         <v>455</v>
       </c>
-      <c r="E260">
+      <c r="E261">
         <v>40479589</v>
       </c>
-      <c r="F260" s="1" t="s">
+      <c r="F261" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="I260" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="261" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A261">
+      <c r="I261" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A262">
         <v>40481901000</v>
       </c>
-      <c r="B261">
+      <c r="B262">
         <v>432571000</v>
       </c>
-      <c r="C261">
+      <c r="C262">
         <v>40481901000</v>
       </c>
-      <c r="D261" t="s">
+      <c r="D262" t="s">
         <v>457</v>
       </c>
-      <c r="E261">
+      <c r="E262">
         <v>40481901</v>
       </c>
-      <c r="F261" s="1" t="s">
+      <c r="F262" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="I261" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="262" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A262">
-        <v>37311061000</v>
-      </c>
-      <c r="B262">
-        <v>37311061000</v>
-      </c>
-      <c r="C262">
-        <v>37311061000</v>
-      </c>
-      <c r="D262" t="s">
-        <v>453</v>
-      </c>
-      <c r="E262">
-        <v>37311061</v>
-      </c>
-      <c r="F262" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="263" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I262" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A263">
-        <v>40490918000</v>
+        <v>40481902000</v>
       </c>
       <c r="B263">
-        <v>432571000</v>
+        <v>40481902000</v>
       </c>
       <c r="C263">
-        <v>40490918000</v>
+        <v>40481902000</v>
       </c>
       <c r="D263" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E263">
-        <v>40490918</v>
+        <v>40481902</v>
       </c>
       <c r="F263" s="1" t="s">
-        <v>516</v>
+        <v>459</v>
       </c>
       <c r="H263" t="s">
-        <v>24</v>
-      </c>
-      <c r="I263" t="s">
-        <v>22</v>
+        <v>460</v>
       </c>
     </row>
     <row r="264" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A264">
+        <v>40490918000</v>
+      </c>
+      <c r="B264">
+        <v>432571000</v>
+      </c>
+      <c r="C264">
+        <v>40490918000</v>
+      </c>
+      <c r="D264" t="s">
+        <v>461</v>
+      </c>
+      <c r="E264">
+        <v>40490918</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="H264" t="s">
+        <v>24</v>
+      </c>
+      <c r="I264" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A265">
         <v>42535714000</v>
       </c>
-      <c r="B264">
+      <c r="B265">
         <v>4137275000</v>
       </c>
-      <c r="C264">
+      <c r="C265">
         <v>42535714000</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D265" t="s">
         <v>462</v>
       </c>
-      <c r="E264">
+      <c r="E265">
         <v>42535714</v>
       </c>
-      <c r="F264" s="1" t="s">
+      <c r="F265" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="I264" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="265" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A265">
-        <v>40481902000</v>
-      </c>
-      <c r="B265">
-        <v>40481902000</v>
-      </c>
-      <c r="C265">
-        <v>40481902000</v>
-      </c>
-      <c r="D265" t="s">
-        <v>458</v>
-      </c>
-      <c r="E265">
-        <v>40481902</v>
-      </c>
-      <c r="F265" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="H265" t="s">
-        <v>460</v>
+      <c r="I265" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="266" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -8387,50 +8387,50 @@
         <v>465</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267">
+        <v>43021226000</v>
+      </c>
+      <c r="B267">
+        <v>43021226000</v>
+      </c>
+      <c r="C267">
+        <v>43021226000</v>
+      </c>
+      <c r="D267" t="s">
+        <v>552</v>
+      </c>
+      <c r="E267">
+        <v>43021226</v>
+      </c>
+      <c r="F267" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H267" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A268">
         <v>43530714000</v>
       </c>
-      <c r="B267">
+      <c r="B268">
         <v>4094294000</v>
       </c>
-      <c r="C267">
+      <c r="C268">
         <v>43530714000</v>
       </c>
-      <c r="D267" t="s">
+      <c r="D268" t="s">
         <v>466</v>
       </c>
-      <c r="E267">
+      <c r="E268">
         <v>43530714</v>
       </c>
-      <c r="F267" s="1" t="s">
+      <c r="F268" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="I267" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A268">
-        <v>43021226000</v>
-      </c>
-      <c r="B268">
-        <v>43021226000</v>
-      </c>
-      <c r="C268">
-        <v>43021226000</v>
-      </c>
-      <c r="D268" t="s">
-        <v>552</v>
-      </c>
-      <c r="E268">
-        <v>43021226</v>
-      </c>
-      <c r="F268" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="H268" t="s">
-        <v>488</v>
+      <c r="I268" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="269" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -8456,55 +8456,55 @@
         <v>469</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A270">
+        <v>45763653000</v>
+      </c>
+      <c r="B270">
+        <v>45763653000</v>
+      </c>
+      <c r="C270">
+        <v>45763653000</v>
+      </c>
+      <c r="D270" t="s">
+        <v>470</v>
+      </c>
+      <c r="E270">
+        <v>45763653</v>
+      </c>
+      <c r="F270" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="H270" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+      <c r="A271">
         <v>46271022000</v>
       </c>
-      <c r="B270">
+      <c r="B271">
         <v>4030518000</v>
       </c>
-      <c r="C270">
+      <c r="C271">
         <v>46271022000</v>
       </c>
-      <c r="D270" t="s">
+      <c r="D271" t="s">
         <v>472</v>
       </c>
-      <c r="E270">
+      <c r="E271">
         <v>46271022</v>
       </c>
-      <c r="F270" s="1" t="s">
+      <c r="F271" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="I270" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="271" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A271">
-        <v>45763653000</v>
-      </c>
-      <c r="B271">
-        <v>45763653000</v>
-      </c>
-      <c r="C271">
-        <v>45763653000</v>
-      </c>
-      <c r="D271" t="s">
-        <v>470</v>
-      </c>
-      <c r="E271">
-        <v>45763653</v>
-      </c>
-      <c r="F271" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="H271" t="s">
-        <v>24</v>
+      <c r="I271" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I271">
-    <sortState ref="A3:I271">
+    <sortState ref="A2:I271">
       <sortCondition ref="C1:C271"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Adding FDA AESI list for Covid vaccine
</commit_message>
<xml_diff>
--- a/extras/PhenotypeDescription.xlsx
+++ b/extras/PhenotypeDescription.xlsx
@@ -2561,9 +2561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="A1:I271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
removed double spaces and NA
</commit_message>
<xml_diff>
--- a/extras/PhenotypeDescription.xlsx
+++ b/extras/PhenotypeDescription.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="566">
   <si>
     <t>oldPhenotypeId</t>
   </si>
@@ -1721,6 +1721,9 @@
   </si>
   <si>
     <t>Overview: [Deprecate in favor of Inflammatory disorder of mediastinum 4189294000] Inflammation of the pericardial fibroelastic sac - classified into five subtypes, Acute and recurrent pericarditis, Pericardial effusion without major hemodynamic compromise, Cardiac tamponade with hemodynamic compromise, Constrictive pericarditis, Effusive-constrictive pericarditis. If myocardial inflammation is also present  then the term myopericarditis or perimyocarditis is used. Presentation: Sharp chest pain improved by sitting up and leaning forward. If pericardiatis is due to infection, fever may be present. Assessment: Auscultation for pericardial friction rub; ECG showing widespread ST elevations, chest x ray, cardiac markers (troponin) elevation, pericardiocentesis/pericardial biopsy, CBC, sed rate, CRP, echocardiography. Blood cultures for fever, rheumatology workup in young women. Plan: NSAIDs (nonsteroidal anti-inflammatory drugs) with colchicine or aspirin. If this treatment fails, further workup needed to rule out atypical forms of pericarditis including tuberculosis, cancer, and inflammatory disease. Most low risk patients may be managed in ambulatory settings, high risk patients need to be hospitalized. High risk features include fever, sub-acute onset, hemodynamic compromise/cardiac tamponade, immunosuppression, on anticoagulant therapy, acute trauma, elevated cardiac enzymes. Prognosis: Patients with acute idiopathic or viral pericarditis have a good long-term prognosis - typically self-limited over 2 weeks with NSAID treatment resulting in good long-term prognosis. Cardiac tamponade rarely occurs in patients with acute idiopathic pericarditis and is more common in patients with a specific underlying etiology such as malignancy, tuberculosis, or purulent pericarditis. Constrictive pericarditis may occur in approximately 1 percent of patients with acute idiopathic pericarditis and is also more common in patients with a specific etiology.</t>
+  </si>
+  <si>
+    <t>Autism spectrum disorder</t>
   </si>
 </sst>
 </file>
@@ -2561,9 +2564,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="A1:I271"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6074,8 +6077,8 @@
       <c r="C160">
         <v>439776000</v>
       </c>
-      <c r="D160">
-        <v>0</v>
+      <c r="D160" t="s">
+        <v>565</v>
       </c>
       <c r="E160">
         <v>439776</v>

</xml_diff>

<commit_message>
removed 440703000,Trigeminal nerve disorder as no cohorts
</commit_message>
<xml_diff>
--- a/extras/PhenotypeDescription.xlsx
+++ b/extras/PhenotypeDescription.xlsx
@@ -15,14 +15,14 @@
     <sheet name="PhenotypeDescription" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PhenotypeDescription!$A$1:$I$271</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PhenotypeDescription!$A$1:$I$270</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="564">
   <si>
     <t>oldPhenotypeId</t>
   </si>
@@ -907,12 +907,6 @@
   </si>
   <si>
     <t>Overview: Pain and inflammation occur when too much uric acid crystallizes and deposits in the joints. Form of arthritis. Gout occurs when urate crystals accumulate in your joint, causing the inflammation and intense pain of a gout attackPresentation: Sudden, severe attacks of pain, swelling, redness and tenderness in the joints, often the joint at the base of the big toe. Symptoms come and go. Tophi - large, visible bumps made of urate crystals. Assessment: joint fluid test (from the affected joint), blood levels of uric acid and creatinine, xray, ultrasound, sual energy CT scan Plan: NSAIDs, Colchicine, Corticosteroids; xanthine oxidase inhibitors (XOIs) and uricosurics to prevent gout complications Prognosis: Early gout diagnosis, therapy enables most patients to live a normal life. Gout is a highly treatable form of arthritis.</t>
-  </si>
-  <si>
-    <t>Trigeminal nerve disorder</t>
-  </si>
-  <si>
-    <t>Overview: Trigeminal (fifth) nerve, largest of the cranial nerve - supplies sensation to the skin of the face and anterior half of head. Motor component - muscles of mastication and tensor tympani of middle ear hearing. Most commonly disorder is Trigeminal neuralgia (tic douloureux) TN - mainly due to compression of the trigeminal nerve root, demyelination (multiple sclerosis). Trigemenial nerve disorder may also present without pain, e.g. trigeminal neuropathy with sensory loss on the face, with weakness of muscles of masticatio- deviation of jaw on opening. Presentation: TN is characterized by recurrent brief episodes of excruciating unilateral electric shock like pain in the lips, gums, cheek or chin. TN is mosstly clustered among middle-aged and elderly persons are affected, with ~ 60% in women. Assessment: TN is a clinical diagnosis - but detailed investigation using neuroimaging to identify cause. Rule out herpes zoster, post traumatic.  Plan: carbamazepine or oxcarbazepine is first line. Gabapentin for non responders. Lidocaine, phenytoin for rescue therapy. Occassionally surgery (gamma knife radiosurgery, rhizotomy, microvascular decompression). Prognosis: highly variable, may go into months of remission. recurrence is common.</t>
   </si>
   <si>
     <t>Takayasu's disease</t>
@@ -2562,11 +2556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I271"/>
+  <dimension ref="A1:I270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A167" sqref="A167:XFD167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2627,7 +2621,7 @@
         <v>24134</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
@@ -2670,7 +2664,7 @@
         <v>27918</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
@@ -2693,7 +2687,7 @@
         <v>30753</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
@@ -2716,7 +2710,7 @@
         <v>31317</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -2739,7 +2733,7 @@
         <v>31967</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="I7" t="s">
         <v>22</v>
@@ -2785,7 +2779,7 @@
         <v>287</v>
       </c>
       <c r="H9" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2805,7 +2799,7 @@
         <v>75860</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="I10" t="s">
         <v>22</v>
@@ -2851,7 +2845,7 @@
         <v>77074</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H12" t="s">
         <v>24</v>
@@ -2900,7 +2894,7 @@
         <v>80182</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -2983,7 +2977,7 @@
         <v>81893</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I18" t="s">
         <v>22</v>
@@ -3006,7 +3000,7 @@
         <v>81902</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -3089,7 +3083,7 @@
         <v>132797</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I23" t="s">
         <v>22</v>
@@ -3112,7 +3106,7 @@
         <v>133169</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I24" t="s">
         <v>22</v>
@@ -3218,7 +3212,7 @@
         <v>137977</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="I29" t="s">
         <v>22</v>
@@ -3281,7 +3275,7 @@
         <v>138994</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="I32" t="s">
         <v>22</v>
@@ -3367,7 +3361,7 @@
         <v>140352</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I36" t="s">
         <v>22</v>
@@ -3470,7 +3464,7 @@
         <v>192359</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I41" t="s">
         <v>22</v>
@@ -3556,7 +3550,7 @@
         <v>194133</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="I45" t="s">
         <v>22</v>
@@ -3599,7 +3593,7 @@
         <v>194992</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I47" t="s">
         <v>22</v>
@@ -3622,7 +3616,7 @@
         <v>196523</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="I48" t="s">
         <v>22</v>
@@ -3797,7 +3791,7 @@
         <v>200219</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="I56" t="s">
         <v>22</v>
@@ -3869,7 +3863,7 @@
         <v>201254</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I59" t="s">
         <v>22</v>
@@ -3892,7 +3886,7 @@
         <v>201340</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I60" t="s">
         <v>22</v>
@@ -3915,7 +3909,7 @@
         <v>201606</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I61" t="s">
         <v>22</v>
@@ -3949,7 +3943,7 @@
         <v>201820000</v>
       </c>
       <c r="D63" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E63">
         <v>201820</v>
@@ -3958,7 +3952,7 @@
         <v>287</v>
       </c>
       <c r="H63" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -3978,7 +3972,7 @@
         <v>201826</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I64" t="s">
         <v>22</v>
@@ -4044,7 +4038,7 @@
         <v>254761</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="I67" t="s">
         <v>22</v>
@@ -4150,7 +4144,7 @@
         <v>312327</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="I72" t="s">
         <v>22</v>
@@ -4173,7 +4167,7 @@
         <v>312437</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="I73" t="s">
         <v>22</v>
@@ -4216,7 +4210,7 @@
         <v>313217</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I75" t="s">
         <v>22</v>
@@ -4239,7 +4233,7 @@
         <v>313223</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I76" t="s">
         <v>22</v>
@@ -4262,7 +4256,7 @@
         <v>313459</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="210" x14ac:dyDescent="0.25">
@@ -4325,7 +4319,7 @@
         <v>314383</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="I80" t="s">
         <v>22</v>
@@ -4394,7 +4388,7 @@
         <v>317009</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="I83" t="s">
         <v>22</v>
@@ -4417,7 +4411,7 @@
         <v>317576</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I84" t="s">
         <v>22</v>
@@ -4572,7 +4566,7 @@
         <v>321042</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H91" t="s">
         <v>24</v>
@@ -4621,7 +4615,7 @@
         <v>321318</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I93" t="s">
         <v>22</v>
@@ -4664,7 +4658,7 @@
         <v>321588</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H95" t="s">
         <v>24</v>
@@ -4710,7 +4704,7 @@
         <v>373503</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I97" t="s">
         <v>22</v>
@@ -4759,7 +4753,7 @@
         <v>374028</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I99" t="s">
         <v>22</v>
@@ -4802,7 +4796,7 @@
         <v>374377</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H101" t="s">
         <v>24</v>
@@ -5006,7 +5000,7 @@
         <v>378253</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="I110" t="s">
         <v>22</v>
@@ -5029,7 +5023,7 @@
         <v>378414</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I111" t="s">
         <v>22</v>
@@ -5092,7 +5086,7 @@
         <v>380378</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I114" t="s">
         <v>22</v>
@@ -5218,7 +5212,7 @@
         <v>432571000</v>
       </c>
       <c r="D120" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E120">
         <v>432571000</v>
@@ -5267,7 +5261,7 @@
         <v>432595</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5330,7 +5324,7 @@
         <v>432870</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I125" t="s">
         <v>22</v>
@@ -5399,7 +5393,7 @@
         <v>433595</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="I128" t="s">
         <v>22</v>
@@ -5502,7 +5496,7 @@
         <v>434592</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I133" t="s">
         <v>22</v>
@@ -5657,7 +5651,7 @@
         <v>248</v>
       </c>
       <c r="H140" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5677,7 +5671,7 @@
         <v>436096</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I141" t="s">
         <v>22</v>
@@ -5720,7 +5714,7 @@
         <v>4307095</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I143" t="s">
         <v>22</v>
@@ -5806,7 +5800,7 @@
         <v>436962</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="I147" t="s">
         <v>22</v>
@@ -5829,7 +5823,7 @@
         <v>437082</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="I148" t="s">
         <v>22</v>
@@ -5895,7 +5889,7 @@
         <v>437312</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I151" t="s">
         <v>22</v>
@@ -5938,7 +5932,7 @@
         <v>437663</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H153" t="s">
         <v>269</v>
@@ -6078,7 +6072,7 @@
         <v>439776000</v>
       </c>
       <c r="D160" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E160">
         <v>439776</v>
@@ -6150,7 +6144,7 @@
         <v>440377</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H163" t="s">
         <v>24</v>
@@ -6221,62 +6215,62 @@
     </row>
     <row r="167" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>440703000</v>
+        <v>440740000</v>
       </c>
       <c r="B167">
-        <v>440703000</v>
+        <v>4137275000</v>
       </c>
       <c r="C167">
-        <v>440703000</v>
+        <v>440740000</v>
       </c>
       <c r="D167" t="s">
         <v>295</v>
       </c>
       <c r="E167">
-        <v>440703</v>
+        <v>440740</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="I167" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>440740000</v>
+        <v>440925000</v>
       </c>
       <c r="B168">
-        <v>4137275000</v>
+        <v>440925000</v>
       </c>
       <c r="C168">
-        <v>440740000</v>
+        <v>440925000</v>
       </c>
       <c r="D168" t="s">
         <v>297</v>
       </c>
       <c r="E168">
-        <v>440740</v>
+        <v>440925</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="I168" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>440925000</v>
+        <v>440940000</v>
       </c>
       <c r="B169">
-        <v>440925000</v>
+        <v>440940000</v>
       </c>
       <c r="C169">
-        <v>440925000</v>
+        <v>440940000</v>
       </c>
       <c r="D169" t="s">
         <v>299</v>
       </c>
       <c r="E169">
-        <v>440925</v>
+        <v>440940</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>300</v>
@@ -6284,151 +6278,154 @@
     </row>
     <row r="170" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>440940000</v>
+        <v>441202000</v>
       </c>
       <c r="B170">
-        <v>440940000</v>
+        <v>43021226000</v>
       </c>
       <c r="C170">
-        <v>440940000</v>
-      </c>
-      <c r="D170" t="s">
+        <v>441202000</v>
+      </c>
+      <c r="D170" s="2" t="s">
         <v>301</v>
       </c>
       <c r="E170">
-        <v>440940</v>
+        <v>441202</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="I170" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>441202000</v>
+        <v>441284000</v>
       </c>
       <c r="B171">
-        <v>43021226000</v>
+        <v>441284000</v>
       </c>
       <c r="C171">
-        <v>441202000</v>
-      </c>
-      <c r="D171" s="2" t="s">
+        <v>441284000</v>
+      </c>
+      <c r="D171" t="s">
         <v>303</v>
       </c>
       <c r="E171">
-        <v>441202</v>
+        <v>441284</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="I171" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>441284000</v>
+        <v>441408000</v>
       </c>
       <c r="B172">
-        <v>441284000</v>
+        <v>4094294000</v>
       </c>
       <c r="C172">
-        <v>441284000</v>
+        <v>441408000</v>
       </c>
       <c r="D172" t="s">
         <v>305</v>
       </c>
       <c r="E172">
-        <v>441284</v>
+        <v>441408</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+      <c r="I172" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>441408000</v>
+        <v>441542000</v>
       </c>
       <c r="B173">
         <v>4094294000</v>
       </c>
       <c r="C173">
-        <v>441408000</v>
+        <v>441542000</v>
       </c>
       <c r="D173" t="s">
+        <v>306</v>
+      </c>
+      <c r="E173">
+        <v>441542</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="I173" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>441788000</v>
+      </c>
+      <c r="B174">
+        <v>441788000</v>
+      </c>
+      <c r="C174">
+        <v>441788000</v>
+      </c>
+      <c r="D174" t="s">
         <v>307</v>
       </c>
-      <c r="E173">
-        <v>441408</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="I173" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A174">
-        <v>441542000</v>
-      </c>
-      <c r="B174">
-        <v>4094294000</v>
-      </c>
-      <c r="C174">
-        <v>441542000</v>
-      </c>
-      <c r="D174" t="s">
+      <c r="E174">
+        <v>441788</v>
+      </c>
+      <c r="F174" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="E174">
-        <v>441542</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="I174" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>441788000</v>
+        <v>441848000</v>
       </c>
       <c r="B175">
-        <v>441788000</v>
+        <v>0</v>
       </c>
       <c r="C175">
-        <v>441788000</v>
+        <v>441848000</v>
       </c>
       <c r="D175" t="s">
         <v>309</v>
       </c>
       <c r="E175">
-        <v>441788</v>
+        <v>441848</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I175" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>441848000</v>
+        <v>442752000</v>
       </c>
       <c r="B176">
-        <v>0</v>
+        <v>4094294000</v>
       </c>
       <c r="C176">
-        <v>441848000</v>
+        <v>442752000</v>
       </c>
       <c r="D176" t="s">
         <v>311</v>
       </c>
       <c r="E176">
-        <v>441848</v>
+        <v>442752</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>312</v>
+        <v>543</v>
       </c>
       <c r="I176" t="s">
         <v>22</v>
@@ -6436,42 +6433,39 @@
     </row>
     <row r="177" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>442752000</v>
+        <v>443213000</v>
       </c>
       <c r="B177">
-        <v>4094294000</v>
+        <v>443213000</v>
       </c>
       <c r="C177">
-        <v>442752000</v>
+        <v>443213000</v>
       </c>
       <c r="D177" t="s">
+        <v>312</v>
+      </c>
+      <c r="E177">
+        <v>443213</v>
+      </c>
+      <c r="F177" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="E177">
-        <v>442752</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="I177" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>443213000</v>
+        <v>443387000</v>
       </c>
       <c r="B178">
-        <v>443213000</v>
+        <v>443387000</v>
       </c>
       <c r="C178">
-        <v>443213000</v>
+        <v>443387000</v>
       </c>
       <c r="D178" t="s">
         <v>314</v>
       </c>
       <c r="E178">
-        <v>443213</v>
+        <v>443387</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>315</v>
@@ -6479,693 +6473,696 @@
     </row>
     <row r="179" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>443387000</v>
+        <v>443392000</v>
       </c>
       <c r="B179">
-        <v>443387000</v>
+        <v>443392000</v>
       </c>
       <c r="C179">
-        <v>443387000</v>
-      </c>
-      <c r="D179" t="s">
+        <v>443392000</v>
+      </c>
+      <c r="D179" s="3" t="s">
         <v>316</v>
       </c>
       <c r="E179">
-        <v>443387</v>
+        <v>443392</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>443392000</v>
+        <v>443454000</v>
       </c>
       <c r="B180">
-        <v>443392000</v>
+        <v>381591000</v>
       </c>
       <c r="C180">
-        <v>443392000</v>
-      </c>
-      <c r="D180" s="3" t="s">
+        <v>443454000</v>
+      </c>
+      <c r="D180" t="s">
         <v>318</v>
       </c>
       <c r="E180">
-        <v>443392</v>
+        <v>443454</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="I180" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>443454000</v>
+        <v>443700000</v>
       </c>
       <c r="B181">
-        <v>381591000</v>
+        <v>443700000</v>
       </c>
       <c r="C181">
-        <v>443454000</v>
+        <v>443700000</v>
       </c>
       <c r="D181" t="s">
         <v>320</v>
       </c>
       <c r="E181">
-        <v>443454</v>
+        <v>443700</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="I181" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>443700000</v>
+        <v>443723000</v>
       </c>
       <c r="B182">
-        <v>443700000</v>
+        <v>443723000</v>
       </c>
       <c r="C182">
-        <v>443700000</v>
+        <v>443723000</v>
       </c>
       <c r="D182" t="s">
+        <v>557</v>
+      </c>
+      <c r="E182">
+        <v>443723</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>443727000</v>
+      </c>
+      <c r="B183">
+        <v>201820000</v>
+      </c>
+      <c r="C183">
+        <v>443727000</v>
+      </c>
+      <c r="D183" t="s">
         <v>322</v>
       </c>
-      <c r="E182">
-        <v>443700</v>
-      </c>
-      <c r="F182" s="1" t="s">
+      <c r="E183">
+        <v>443727</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="I183" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>444044000</v>
+      </c>
+      <c r="B184">
+        <v>4030518000</v>
+      </c>
+      <c r="C184">
+        <v>444044000</v>
+      </c>
+      <c r="D184" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183">
-        <v>443723000</v>
-      </c>
-      <c r="B183">
-        <v>443723000</v>
-      </c>
-      <c r="C183">
-        <v>443723000</v>
-      </c>
-      <c r="D183" t="s">
-        <v>559</v>
-      </c>
-      <c r="E183">
-        <v>443723</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A184">
-        <v>443727000</v>
-      </c>
-      <c r="B184">
-        <v>201820000</v>
-      </c>
-      <c r="C184">
-        <v>443727000</v>
-      </c>
-      <c r="D184" t="s">
+      <c r="E184">
+        <v>444044</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I184" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>444070000</v>
+      </c>
+      <c r="B185">
+        <v>4094294000</v>
+      </c>
+      <c r="C185">
+        <v>444070000</v>
+      </c>
+      <c r="D185" t="s">
         <v>324</v>
       </c>
-      <c r="E184">
-        <v>443727</v>
-      </c>
-      <c r="F184" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="I184" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A185">
-        <v>444044000</v>
-      </c>
-      <c r="B185">
-        <v>4030518000</v>
-      </c>
-      <c r="C185">
-        <v>444044000</v>
-      </c>
-      <c r="D185" t="s">
+      <c r="E185">
+        <v>444070</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="I185" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>444247000</v>
+      </c>
+      <c r="B186">
+        <v>444247000</v>
+      </c>
+      <c r="C186">
+        <v>444247000</v>
+      </c>
+      <c r="D186" t="s">
         <v>325</v>
       </c>
-      <c r="E185">
-        <v>444044</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="I185" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A186">
-        <v>444070000</v>
-      </c>
-      <c r="B186">
-        <v>4094294000</v>
-      </c>
-      <c r="C186">
-        <v>444070000</v>
-      </c>
-      <c r="D186" t="s">
+      <c r="E186">
+        <v>444247</v>
+      </c>
+      <c r="F186" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="E186">
-        <v>444070</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="I186" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>444247000</v>
+        <v>444429000</v>
       </c>
       <c r="B187">
-        <v>444247000</v>
+        <v>444429000</v>
       </c>
       <c r="C187">
-        <v>444247000</v>
+        <v>444429000</v>
       </c>
       <c r="D187" t="s">
         <v>327</v>
       </c>
       <c r="E187">
-        <v>444247</v>
+        <v>444429</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>444429000</v>
+        <v>4000634000</v>
       </c>
       <c r="B188">
-        <v>444429000</v>
+        <v>73553000</v>
       </c>
       <c r="C188">
-        <v>444429000</v>
+        <v>4000634000</v>
       </c>
       <c r="D188" t="s">
         <v>329</v>
       </c>
       <c r="E188">
-        <v>444429</v>
+        <v>4000634</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="H188" t="s">
+        <v>331</v>
+      </c>
+      <c r="I188" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>4000634000</v>
+        <v>4002359000</v>
       </c>
       <c r="B189">
-        <v>73553000</v>
+        <v>436081000</v>
       </c>
       <c r="C189">
-        <v>4000634000</v>
+        <v>4002359000</v>
       </c>
       <c r="D189" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E189">
-        <v>4000634</v>
+        <v>4002359</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="H189" t="s">
         <v>333</v>
       </c>
       <c r="I189" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>4002359000</v>
+        <v>4013643000</v>
       </c>
       <c r="B190">
-        <v>436081000</v>
+        <v>4013643000</v>
       </c>
       <c r="C190">
-        <v>4002359000</v>
+        <v>4013643000</v>
       </c>
       <c r="D190" t="s">
         <v>334</v>
       </c>
       <c r="E190">
-        <v>4002359</v>
+        <v>4013643</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="I190" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>4013643000</v>
+        <v>4024659000</v>
       </c>
       <c r="B191">
-        <v>4013643000</v>
+        <v>201820000</v>
       </c>
       <c r="C191">
-        <v>4013643000</v>
+        <v>4024659000</v>
       </c>
       <c r="D191" t="s">
         <v>336</v>
       </c>
       <c r="E191">
-        <v>4013643</v>
+        <v>4024659</v>
       </c>
       <c r="F191" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="H191" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I191" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>4024659000</v>
+        <v>4027537000</v>
       </c>
       <c r="B192">
-        <v>201820000</v>
+        <v>4027537000</v>
       </c>
       <c r="C192">
-        <v>4024659000</v>
+        <v>4027537000</v>
       </c>
       <c r="D192" t="s">
         <v>338</v>
       </c>
       <c r="E192">
-        <v>4024659</v>
+        <v>4027537</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="H192" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>4028363000</v>
+      </c>
+      <c r="B193">
+        <v>4028363000</v>
+      </c>
+      <c r="C193">
+        <v>4028363000</v>
+      </c>
+      <c r="D193" t="s">
         <v>339</v>
       </c>
-      <c r="I192" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193">
-        <v>4027537000</v>
-      </c>
-      <c r="B193">
-        <v>4027537000</v>
-      </c>
-      <c r="C193">
-        <v>4027537000</v>
-      </c>
-      <c r="D193" t="s">
+      <c r="E193">
+        <v>4028363</v>
+      </c>
+      <c r="F193" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="E193">
-        <v>4027537</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="1:9" ht="375" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>4028363000</v>
+        <v>4030518000</v>
       </c>
       <c r="B194">
-        <v>4028363000</v>
+        <v>4030518000</v>
       </c>
       <c r="C194">
-        <v>4028363000</v>
+        <v>4030518000</v>
       </c>
       <c r="D194" t="s">
         <v>341</v>
       </c>
       <c r="E194">
-        <v>4028363</v>
+        <v>4030518</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>4030518000</v>
+        <v>4038838000</v>
       </c>
       <c r="B195">
-        <v>4030518000</v>
+        <v>432571000</v>
       </c>
       <c r="C195">
-        <v>4030518000</v>
+        <v>4038838000</v>
       </c>
       <c r="D195" t="s">
         <v>343</v>
       </c>
       <c r="E195">
-        <v>4030518</v>
+        <v>4038838</v>
       </c>
       <c r="F195" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="I195" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>4043371000</v>
+      </c>
+      <c r="C196">
+        <v>4043371000</v>
+      </c>
+      <c r="D196" t="s">
+        <v>472</v>
+      </c>
+      <c r="E196">
+        <v>4043371</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H196" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>4046338000</v>
+      </c>
+      <c r="B197">
+        <v>4046338000</v>
+      </c>
+      <c r="C197">
+        <v>4046338000</v>
+      </c>
+      <c r="D197" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A196">
-        <v>4038838000</v>
-      </c>
-      <c r="B196">
-        <v>432571000</v>
-      </c>
-      <c r="C196">
-        <v>4038838000</v>
-      </c>
-      <c r="D196" t="s">
+      <c r="E197">
+        <v>4046338</v>
+      </c>
+      <c r="F197" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="E196">
-        <v>4038838</v>
-      </c>
-      <c r="F196" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="I196" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B197">
-        <v>4043371000</v>
-      </c>
-      <c r="C197">
-        <v>4043371000</v>
-      </c>
-      <c r="D197" t="s">
-        <v>474</v>
-      </c>
-      <c r="E197">
-        <v>4043371</v>
-      </c>
-      <c r="F197" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="H197" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>4046338000</v>
+        <v>4058821000</v>
       </c>
       <c r="B198">
-        <v>4046338000</v>
+        <v>4212540000</v>
       </c>
       <c r="C198">
-        <v>4046338000</v>
+        <v>4058821000</v>
       </c>
       <c r="D198" t="s">
         <v>346</v>
       </c>
       <c r="E198">
-        <v>4046338</v>
+        <v>4058821</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="I198" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>4058821000</v>
+        <v>4063434000</v>
       </c>
       <c r="B199">
+        <v>140168000</v>
+      </c>
+      <c r="C199">
+        <v>4063434000</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E199">
+        <v>4063434</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="I199" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>4064161000</v>
+      </c>
+      <c r="B200">
         <v>4212540000</v>
       </c>
-      <c r="C199">
-        <v>4058821000</v>
-      </c>
-      <c r="D199" t="s">
-        <v>348</v>
-      </c>
-      <c r="E199">
-        <v>4058821</v>
-      </c>
-      <c r="F199" s="1" t="s">
+      <c r="C200">
+        <v>4064161000</v>
+      </c>
+      <c r="D200" t="s">
         <v>349</v>
       </c>
-      <c r="I199" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A200">
-        <v>4063434000</v>
-      </c>
-      <c r="B200">
-        <v>140168000</v>
-      </c>
-      <c r="C200">
-        <v>4063434000</v>
-      </c>
-      <c r="D200" s="3" t="s">
+      <c r="E200">
+        <v>4064161</v>
+      </c>
+      <c r="F200" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="E200">
-        <v>4063434</v>
-      </c>
-      <c r="F200" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="I200" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>4064161000</v>
+        <v>4067106000</v>
       </c>
       <c r="B201">
-        <v>4212540000</v>
+        <v>4067106000</v>
       </c>
       <c r="C201">
-        <v>4064161000</v>
+        <v>4067106000</v>
       </c>
       <c r="D201" t="s">
         <v>351</v>
       </c>
       <c r="E201">
-        <v>4064161</v>
+        <v>4067106</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="I201" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>4067106000</v>
+        <v>4070552000</v>
       </c>
       <c r="B202">
-        <v>4067106000</v>
+        <v>4164770000</v>
       </c>
       <c r="C202">
-        <v>4067106000</v>
+        <v>4070552000</v>
       </c>
       <c r="D202" t="s">
         <v>353</v>
       </c>
       <c r="E202">
-        <v>4067106</v>
+        <v>4070552</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="H202" t="s">
+        <v>355</v>
+      </c>
+      <c r="I202" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>4070552000</v>
+        <v>4074815000</v>
       </c>
       <c r="B203">
-        <v>4164770000</v>
+        <v>4043371000</v>
       </c>
       <c r="C203">
-        <v>4070552000</v>
+        <v>4074815000</v>
       </c>
       <c r="D203" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E203">
-        <v>4070552</v>
+        <v>4074815</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="H203" t="s">
+        <v>478</v>
+      </c>
+      <c r="I203" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>4079843000</v>
+      </c>
+      <c r="B204">
+        <v>4306655000</v>
+      </c>
+      <c r="C204">
+        <v>4079843000</v>
+      </c>
+      <c r="D204" t="s">
         <v>357</v>
       </c>
-      <c r="I203" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A204">
-        <v>4074815000</v>
-      </c>
-      <c r="B204">
-        <v>4043371000</v>
-      </c>
-      <c r="C204">
-        <v>4074815000</v>
-      </c>
-      <c r="D204" t="s">
+      <c r="E204">
+        <v>4079843</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I204" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>4091559000</v>
+      </c>
+      <c r="B205">
+        <v>378135000</v>
+      </c>
+      <c r="C205">
+        <v>4091559000</v>
+      </c>
+      <c r="D205" t="s">
         <v>358</v>
       </c>
-      <c r="E204">
-        <v>4074815</v>
-      </c>
-      <c r="F204" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="I204" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="205" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A205">
-        <v>4079843000</v>
-      </c>
-      <c r="B205">
-        <v>4306655000</v>
-      </c>
-      <c r="C205">
-        <v>4079843000</v>
-      </c>
-      <c r="D205" t="s">
+      <c r="E205">
+        <v>4091559</v>
+      </c>
+      <c r="F205" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="E205">
-        <v>4079843</v>
-      </c>
-      <c r="F205" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="I205" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>4091559000</v>
+        <v>4092289000</v>
       </c>
       <c r="B206">
-        <v>378135000</v>
+        <v>4092289000</v>
       </c>
       <c r="C206">
-        <v>4091559000</v>
+        <v>4092289000</v>
       </c>
       <c r="D206" t="s">
         <v>360</v>
       </c>
       <c r="E206">
-        <v>4091559</v>
+        <v>4092289</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="I206" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="207" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>4092289000</v>
+        <v>4094294000</v>
       </c>
       <c r="B207">
-        <v>4092289000</v>
+        <v>4094294000</v>
       </c>
       <c r="C207">
-        <v>4092289000</v>
+        <v>4094294000</v>
       </c>
       <c r="D207" t="s">
+        <v>520</v>
+      </c>
+      <c r="E207">
+        <v>4094294</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>4098292000</v>
+      </c>
+      <c r="B208">
+        <v>4098292000</v>
+      </c>
+      <c r="C208">
+        <v>4098292000</v>
+      </c>
+      <c r="D208" t="s">
         <v>362</v>
       </c>
-      <c r="E207">
-        <v>4092289</v>
-      </c>
-      <c r="F207" s="1" t="s">
+      <c r="E208">
+        <v>4098292</v>
+      </c>
+      <c r="F208" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A208">
-        <v>4094294000</v>
-      </c>
-      <c r="B208">
-        <v>4094294000</v>
-      </c>
-      <c r="C208">
-        <v>4094294000</v>
-      </c>
-      <c r="D208" t="s">
-        <v>522</v>
-      </c>
-      <c r="E208">
-        <v>4094294</v>
-      </c>
-      <c r="F208" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>4098292000</v>
+        <v>4098597000</v>
       </c>
       <c r="B209">
-        <v>4098292000</v>
+        <v>436081000</v>
       </c>
       <c r="C209">
-        <v>4098292000</v>
+        <v>4098597000</v>
       </c>
       <c r="D209" t="s">
         <v>364</v>
       </c>
       <c r="E209">
-        <v>4098292</v>
+        <v>4098597</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="I209" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>4098597000</v>
+        <v>4101602000</v>
       </c>
       <c r="B210">
-        <v>436081000</v>
+        <v>4137275000</v>
       </c>
       <c r="C210">
-        <v>4098597000</v>
+        <v>4101602000</v>
       </c>
       <c r="D210" t="s">
         <v>366</v>
       </c>
       <c r="E210">
-        <v>4098597</v>
+        <v>4101602</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>367</v>
@@ -7174,864 +7171,861 @@
         <v>22</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>4101602000</v>
+        <v>4103295000</v>
       </c>
       <c r="B211">
-        <v>4137275000</v>
+        <v>44784217000</v>
       </c>
       <c r="C211">
-        <v>4101602000</v>
+        <v>4103295000</v>
       </c>
       <c r="D211" t="s">
         <v>368</v>
       </c>
       <c r="E211">
-        <v>4101602</v>
+        <v>4103295</v>
       </c>
       <c r="F211" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="I211" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>4112853000</v>
+      </c>
+      <c r="B212">
+        <v>4112853000</v>
+      </c>
+      <c r="C212">
+        <v>4112853000</v>
+      </c>
+      <c r="D212" t="s">
         <v>369</v>
       </c>
-      <c r="I211" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="212" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A212">
-        <v>4103295000</v>
-      </c>
-      <c r="B212">
-        <v>44784217000</v>
-      </c>
-      <c r="C212">
-        <v>4103295000</v>
-      </c>
-      <c r="D212" t="s">
+      <c r="E212">
+        <v>4112853</v>
+      </c>
+      <c r="F212" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="E212">
-        <v>4103295</v>
-      </c>
-      <c r="F212" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="I212" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="213" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>4112853000</v>
+        <v>4124836000</v>
       </c>
       <c r="B213">
-        <v>4112853000</v>
+        <v>321052000</v>
       </c>
       <c r="C213">
-        <v>4112853000</v>
+        <v>4124836000</v>
       </c>
       <c r="D213" t="s">
         <v>371</v>
       </c>
       <c r="E213">
-        <v>4112853</v>
+        <v>4124836</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>372</v>
       </c>
+      <c r="I213" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="214" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>4124836000</v>
+        <v>4131909000</v>
       </c>
       <c r="B214">
-        <v>321052000</v>
+        <v>4131909000</v>
       </c>
       <c r="C214">
-        <v>4124836000</v>
+        <v>4131909000</v>
       </c>
       <c r="D214" t="s">
         <v>373</v>
       </c>
       <c r="E214">
-        <v>4124836</v>
+        <v>4131909</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I214" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="215" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>4131909000</v>
+        <v>4133004000</v>
       </c>
       <c r="B215">
-        <v>4131909000</v>
+        <v>4133004000</v>
       </c>
       <c r="C215">
-        <v>4131909000</v>
+        <v>4133004000</v>
       </c>
       <c r="D215" t="s">
         <v>375</v>
       </c>
       <c r="E215">
-        <v>4131909</v>
+        <v>4133004</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>4133004000</v>
+        <v>4137275000</v>
       </c>
       <c r="B216">
-        <v>4133004000</v>
+        <v>4137275000</v>
       </c>
       <c r="C216">
-        <v>4133004000</v>
+        <v>4137275000</v>
       </c>
       <c r="D216" t="s">
         <v>377</v>
       </c>
       <c r="E216">
-        <v>4133004</v>
+        <v>4137275</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>4137275000</v>
+        <v>4138837000</v>
       </c>
       <c r="B217">
-        <v>4137275000</v>
+        <v>4189294000</v>
       </c>
       <c r="C217">
-        <v>4137275000</v>
+        <v>4138837000</v>
       </c>
       <c r="D217" t="s">
         <v>379</v>
       </c>
       <c r="E217">
-        <v>4137275</v>
+        <v>4138837</v>
       </c>
       <c r="F217" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="H217" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="218" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="I217" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>4138837000</v>
+        <v>4139034000</v>
       </c>
       <c r="B218">
-        <v>4189294000</v>
+        <v>4139034000</v>
       </c>
       <c r="C218">
-        <v>4138837000</v>
+        <v>4139034000</v>
       </c>
       <c r="D218" t="s">
         <v>381</v>
       </c>
       <c r="E218">
-        <v>4138837</v>
+        <v>4139034</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>564</v>
+        <v>382</v>
       </c>
       <c r="H218" t="s">
-        <v>382</v>
-      </c>
-      <c r="I218" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="219" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>4139034000</v>
+        <v>4147411000</v>
       </c>
       <c r="B219">
-        <v>4139034000</v>
+        <v>432571000</v>
       </c>
       <c r="C219">
-        <v>4139034000</v>
+        <v>4147411000</v>
       </c>
       <c r="D219" t="s">
         <v>383</v>
       </c>
       <c r="E219">
-        <v>4139034</v>
+        <v>4147411</v>
       </c>
       <c r="F219" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="I219" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>4163261000</v>
+      </c>
+      <c r="B220">
+        <v>4163261000</v>
+      </c>
+      <c r="C220">
+        <v>4163261000</v>
+      </c>
+      <c r="D220" t="s">
         <v>384</v>
       </c>
-      <c r="H219" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="220" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A220">
-        <v>4147411000</v>
-      </c>
-      <c r="B220">
-        <v>432571000</v>
-      </c>
-      <c r="C220">
-        <v>4147411000</v>
-      </c>
-      <c r="D220" t="s">
+      <c r="E220">
+        <v>4163261</v>
+      </c>
+      <c r="F220" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E220">
-        <v>4147411</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="I220" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>4163261000</v>
+        <v>4164770000</v>
       </c>
       <c r="B221">
-        <v>4163261000</v>
+        <v>4164770000</v>
       </c>
       <c r="C221">
-        <v>4163261000</v>
+        <v>4164770000</v>
       </c>
       <c r="D221" t="s">
         <v>386</v>
       </c>
       <c r="E221">
-        <v>4163261</v>
+        <v>4164770</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>4164770000</v>
+        <v>4169095000</v>
       </c>
       <c r="B222">
-        <v>4164770000</v>
+        <v>4094294000</v>
       </c>
       <c r="C222">
-        <v>4164770000</v>
+        <v>4169095000</v>
       </c>
       <c r="D222" t="s">
         <v>388</v>
       </c>
       <c r="E222">
-        <v>4164770</v>
+        <v>4169095</v>
       </c>
       <c r="F222" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="I222" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>4174977000</v>
+      </c>
+      <c r="B223">
+        <v>378416000</v>
+      </c>
+      <c r="C223">
+        <v>4174977000</v>
+      </c>
+      <c r="D223" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="223" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A223">
-        <v>4169095000</v>
-      </c>
-      <c r="B223">
-        <v>4094294000</v>
-      </c>
-      <c r="C223">
-        <v>4169095000</v>
-      </c>
-      <c r="D223" t="s">
+      <c r="E223">
+        <v>4174977</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I223" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>4175485000</v>
+      </c>
+      <c r="C224">
+        <v>4175485000</v>
+      </c>
+      <c r="D224" t="s">
+        <v>502</v>
+      </c>
+      <c r="E224">
+        <v>4175485</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>4180790000</v>
+      </c>
+      <c r="B225">
+        <v>4180790000</v>
+      </c>
+      <c r="C225">
+        <v>4180790000</v>
+      </c>
+      <c r="D225" t="s">
         <v>390</v>
       </c>
-      <c r="E223">
-        <v>4169095</v>
-      </c>
-      <c r="F223" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="I223" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="224" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A224">
-        <v>4174977000</v>
-      </c>
-      <c r="B224">
-        <v>378416000</v>
-      </c>
-      <c r="C224">
-        <v>4174977000</v>
-      </c>
-      <c r="D224" t="s">
+      <c r="E225">
+        <v>4180790</v>
+      </c>
+      <c r="F225" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="E224">
-        <v>4174977</v>
-      </c>
-      <c r="F224" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="I224" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B225">
-        <v>4175485000</v>
-      </c>
-      <c r="C225">
-        <v>4175485000</v>
-      </c>
-      <c r="D225" t="s">
-        <v>504</v>
-      </c>
-      <c r="E225">
-        <v>4175485</v>
-      </c>
-      <c r="F225" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="226" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="226" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>4180790000</v>
+        <v>4181343000</v>
       </c>
       <c r="B226">
-        <v>4180790000</v>
+        <v>4181343000</v>
       </c>
       <c r="C226">
-        <v>4180790000</v>
+        <v>4181343000</v>
       </c>
       <c r="D226" t="s">
         <v>392</v>
       </c>
       <c r="E226">
-        <v>4180790</v>
+        <v>4181343</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>4181343000</v>
+        <v>4181351000</v>
       </c>
       <c r="B227">
-        <v>4181343000</v>
+        <v>4181351000</v>
       </c>
       <c r="C227">
-        <v>4181343000</v>
+        <v>4181351000</v>
       </c>
       <c r="D227" t="s">
         <v>394</v>
       </c>
       <c r="E227">
-        <v>4181343</v>
+        <v>4181351</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>4181351000</v>
+        <v>4182210000</v>
       </c>
       <c r="B228">
-        <v>4181351000</v>
+        <v>4182210000</v>
       </c>
       <c r="C228">
-        <v>4181351000</v>
+        <v>4182210000</v>
       </c>
       <c r="D228" t="s">
         <v>396</v>
       </c>
       <c r="E228">
-        <v>4181351</v>
+        <v>4182210</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>4182210000</v>
+        <v>4182711000</v>
       </c>
       <c r="B229">
-        <v>4182210000</v>
+        <v>4137275000</v>
       </c>
       <c r="C229">
-        <v>4182210000</v>
+        <v>4182711000</v>
       </c>
       <c r="D229" t="s">
         <v>398</v>
       </c>
       <c r="E229">
-        <v>4182210</v>
+        <v>4182711</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="230" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="H229" t="s">
+        <v>400</v>
+      </c>
+      <c r="I229" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>4182711000</v>
+        <v>4185711000</v>
       </c>
       <c r="B230">
-        <v>4137275000</v>
+        <v>4094294000</v>
       </c>
       <c r="C230">
-        <v>4182711000</v>
+        <v>4185711000</v>
       </c>
       <c r="D230" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E230">
-        <v>4182711</v>
+        <v>4185711</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="H230" t="s">
-        <v>402</v>
+        <v>546</v>
       </c>
       <c r="I230" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>4185711000</v>
+        <v>4185932000</v>
       </c>
       <c r="B231">
-        <v>4094294000</v>
+        <v>4185932000</v>
       </c>
       <c r="C231">
-        <v>4185711000</v>
-      </c>
-      <c r="D231" t="s">
-        <v>403</v>
+        <v>4185932000</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>551</v>
       </c>
       <c r="E231">
-        <v>4185711</v>
+        <v>4185932</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="I231" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="232" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>4185932000</v>
+        <v>4189294000</v>
       </c>
       <c r="B232">
-        <v>4185932000</v>
+        <v>4189294000</v>
       </c>
       <c r="C232">
-        <v>4185932000</v>
-      </c>
-      <c r="D232" s="3" t="s">
-        <v>553</v>
+        <v>4189294000</v>
+      </c>
+      <c r="D232" t="s">
+        <v>560</v>
       </c>
       <c r="E232">
-        <v>4185932</v>
-      </c>
-      <c r="F232" s="1" t="s">
-        <v>554</v>
+        <v>4189294</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>4189294000</v>
+        <v>4190307000</v>
       </c>
       <c r="B233">
-        <v>4189294000</v>
+        <v>4190307000</v>
       </c>
       <c r="C233">
-        <v>4189294000</v>
+        <v>4190307000</v>
       </c>
       <c r="D233" t="s">
-        <v>562</v>
+        <v>402</v>
       </c>
       <c r="E233">
-        <v>4189294</v>
-      </c>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4190307</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A234">
+        <v>4195694000</v>
+      </c>
+      <c r="B234">
+        <v>4195694000</v>
+      </c>
+      <c r="C234">
+        <v>4195694000</v>
+      </c>
+      <c r="D234" t="s">
+        <v>403</v>
+      </c>
+      <c r="E234">
+        <v>4195694</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="H234" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>4201096000</v>
+      </c>
+      <c r="B235">
         <v>4190307000</v>
       </c>
-      <c r="B234">
-        <v>4190307000</v>
-      </c>
-      <c r="C234">
-        <v>4190307000</v>
-      </c>
-      <c r="D234" t="s">
-        <v>404</v>
-      </c>
-      <c r="E234">
-        <v>4190307</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="235" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A235">
-        <v>4195694000</v>
-      </c>
-      <c r="B235">
-        <v>4195694000</v>
-      </c>
       <c r="C235">
-        <v>4195694000</v>
+        <v>4201096000</v>
       </c>
       <c r="D235" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E235">
-        <v>4195694</v>
+        <v>4201096</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="H235" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="236" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="I235" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>4201096000</v>
+        <v>4212540000</v>
       </c>
       <c r="B236">
-        <v>4190307000</v>
+        <v>4212540000</v>
       </c>
       <c r="C236">
-        <v>4201096000</v>
+        <v>4212540000</v>
       </c>
       <c r="D236" t="s">
         <v>408</v>
       </c>
       <c r="E236">
-        <v>4201096</v>
+        <v>4212540</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="I236" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="237" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>4212540000</v>
+        <v>4223659000</v>
       </c>
       <c r="B237">
-        <v>4212540000</v>
+        <v>4094294000</v>
       </c>
       <c r="C237">
-        <v>4212540000</v>
+        <v>4223659000</v>
       </c>
       <c r="D237" t="s">
         <v>410</v>
       </c>
       <c r="E237">
-        <v>4212540</v>
+        <v>4223659</v>
       </c>
       <c r="F237" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="I237" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>4236484000</v>
+      </c>
+      <c r="B238">
+        <v>4236484000</v>
+      </c>
+      <c r="C238">
+        <v>4236484000</v>
+      </c>
+      <c r="D238" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="238" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A238">
-        <v>4223659000</v>
-      </c>
-      <c r="B238">
-        <v>4094294000</v>
-      </c>
-      <c r="C238">
-        <v>4223659000</v>
-      </c>
-      <c r="D238" t="s">
+      <c r="E238">
+        <v>4236484</v>
+      </c>
+      <c r="F238" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="E238">
-        <v>4223659</v>
-      </c>
-      <c r="F238" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="I238" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>4236484000</v>
+        <v>4245975000</v>
       </c>
       <c r="B239">
-        <v>4236484000</v>
+        <v>4245975000</v>
       </c>
       <c r="C239">
-        <v>4236484000</v>
+        <v>4245975000</v>
       </c>
       <c r="D239" t="s">
         <v>413</v>
       </c>
       <c r="E239">
-        <v>4236484</v>
+        <v>4245975</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>4245975000</v>
+        <v>4246127000</v>
       </c>
       <c r="B240">
-        <v>4245975000</v>
+        <v>4246127000</v>
       </c>
       <c r="C240">
-        <v>4245975000</v>
+        <v>4246127000</v>
       </c>
       <c r="D240" t="s">
         <v>415</v>
       </c>
       <c r="E240">
-        <v>4245975</v>
+        <v>4246127</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="241" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="H240" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>4246127000</v>
+        <v>4253901000</v>
       </c>
       <c r="B241">
-        <v>4246127000</v>
+        <v>73553000</v>
       </c>
       <c r="C241">
-        <v>4246127000</v>
+        <v>4253901000</v>
       </c>
       <c r="D241" t="s">
         <v>417</v>
       </c>
       <c r="E241">
-        <v>4246127</v>
+        <v>4253901</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="H241" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="242" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="I241" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>4253901000</v>
+        <v>4256228000</v>
       </c>
       <c r="B242">
-        <v>73553000</v>
+        <v>4256228000</v>
       </c>
       <c r="C242">
-        <v>4253901000</v>
+        <v>4256228000</v>
       </c>
       <c r="D242" t="s">
         <v>419</v>
       </c>
       <c r="E242">
-        <v>4253901</v>
+        <v>4256228</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="I242" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="243" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="H242" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A243">
-        <v>4256228000</v>
+        <v>4260535000</v>
       </c>
       <c r="B243">
-        <v>4256228000</v>
+        <v>4043371000</v>
       </c>
       <c r="C243">
-        <v>4256228000</v>
+        <v>4260535000</v>
       </c>
       <c r="D243" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E243">
-        <v>4256228</v>
+        <v>4260535</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>422</v>
+        <v>479</v>
       </c>
       <c r="H243" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="244" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="I243" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A244">
-        <v>4260535000</v>
+        <v>4266367000</v>
       </c>
       <c r="B244">
-        <v>4043371000</v>
+        <v>4266367000</v>
       </c>
       <c r="C244">
-        <v>4260535000</v>
+        <v>4266367000</v>
       </c>
       <c r="D244" t="s">
         <v>424</v>
       </c>
       <c r="E244">
-        <v>4260535</v>
+        <v>4266367</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="H244" t="s">
         <v>425</v>
       </c>
-      <c r="I244" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="245" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="245" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>4266367000</v>
+        <v>4272240000</v>
       </c>
       <c r="B245">
-        <v>4266367000</v>
+        <v>4094294000</v>
       </c>
       <c r="C245">
-        <v>4266367000</v>
+        <v>4272240000</v>
       </c>
       <c r="D245" t="s">
         <v>426</v>
       </c>
       <c r="E245">
-        <v>4266367</v>
+        <v>4272240</v>
       </c>
       <c r="F245" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="I245" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>4273391000</v>
+      </c>
+      <c r="B246">
+        <v>4273391000</v>
+      </c>
+      <c r="C246">
+        <v>4273391000</v>
+      </c>
+      <c r="D246" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="246" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A246">
-        <v>4272240000</v>
-      </c>
-      <c r="B246">
-        <v>4094294000</v>
-      </c>
-      <c r="C246">
-        <v>4272240000</v>
-      </c>
-      <c r="D246" t="s">
+      <c r="E246">
+        <v>4273391</v>
+      </c>
+      <c r="F246" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="E246">
-        <v>4272240</v>
-      </c>
-      <c r="F246" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="I246" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="247" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>4273391000</v>
+        <v>4281232000</v>
       </c>
       <c r="B247">
-        <v>4273391000</v>
+        <v>4212540000</v>
       </c>
       <c r="C247">
-        <v>4273391000</v>
+        <v>4281232000</v>
       </c>
       <c r="D247" t="s">
         <v>429</v>
       </c>
       <c r="E247">
-        <v>4273391</v>
+        <v>4281232</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="248" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="I247" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A248">
-        <v>4281232000</v>
+        <v>4284492000</v>
       </c>
       <c r="B248">
-        <v>4212540000</v>
+        <v>140168000</v>
       </c>
       <c r="C248">
-        <v>4281232000</v>
-      </c>
-      <c r="D248" t="s">
+        <v>4284492000</v>
+      </c>
+      <c r="D248" s="3" t="s">
         <v>431</v>
       </c>
       <c r="E248">
-        <v>4281232</v>
+        <v>4284492</v>
       </c>
       <c r="F248" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="I248" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>4285717000</v>
+      </c>
+      <c r="B249">
+        <v>4285717000</v>
+      </c>
+      <c r="C249">
+        <v>4285717000</v>
+      </c>
+      <c r="D249" t="s">
         <v>432</v>
       </c>
-      <c r="I248" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="249" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A249">
-        <v>4284492000</v>
-      </c>
-      <c r="B249">
-        <v>140168000</v>
-      </c>
-      <c r="C249">
-        <v>4284492000</v>
-      </c>
-      <c r="D249" s="3" t="s">
+      <c r="E249">
+        <v>4285717</v>
+      </c>
+      <c r="F249" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="E249">
-        <v>4284492</v>
-      </c>
-      <c r="F249" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="I249" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="250" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="250" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A250">
-        <v>4285717000</v>
+        <v>4286201000</v>
       </c>
       <c r="B250">
-        <v>4285717000</v>
+        <v>4286201000</v>
       </c>
       <c r="C250">
-        <v>4285717000</v>
+        <v>4286201000</v>
       </c>
       <c r="D250" t="s">
         <v>434</v>
       </c>
       <c r="E250">
-        <v>4285717</v>
+        <v>4286201</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>435</v>
@@ -8039,237 +8033,240 @@
     </row>
     <row r="251" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>4286201000</v>
+        <v>4290976000</v>
       </c>
       <c r="B251">
-        <v>4286201000</v>
+        <v>4137275000</v>
       </c>
       <c r="C251">
-        <v>4286201000</v>
+        <v>4290976000</v>
       </c>
       <c r="D251" t="s">
         <v>436</v>
       </c>
       <c r="E251">
-        <v>4286201</v>
+        <v>4290976</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="252" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="I251" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>4290976000</v>
+        <v>4299535000</v>
       </c>
       <c r="B252">
-        <v>4137275000</v>
+        <v>4299535000</v>
       </c>
       <c r="C252">
-        <v>4290976000</v>
+        <v>4299535000</v>
       </c>
       <c r="D252" t="s">
         <v>438</v>
       </c>
       <c r="E252">
-        <v>4290976</v>
+        <v>4299535</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="I252" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="253" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253">
-        <v>4299535000</v>
+        <v>4306655000</v>
       </c>
       <c r="B253">
-        <v>4299535000</v>
+        <v>4306655000</v>
       </c>
       <c r="C253">
-        <v>4299535000</v>
+        <v>4306655000</v>
       </c>
       <c r="D253" t="s">
         <v>440</v>
       </c>
       <c r="E253">
-        <v>4299535</v>
+        <v>4306655</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A254">
-        <v>4306655000</v>
+        <v>4311499000</v>
       </c>
       <c r="B254">
-        <v>4306655000</v>
+        <v>4311499000</v>
       </c>
       <c r="C254">
-        <v>4306655000</v>
+        <v>4311499000</v>
       </c>
       <c r="D254" t="s">
         <v>442</v>
       </c>
       <c r="E254">
-        <v>4306655</v>
+        <v>4311499</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="255" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="H254" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A255">
-        <v>4311499000</v>
+        <v>4318985000</v>
       </c>
       <c r="B255">
-        <v>4311499000</v>
+        <v>378416000</v>
       </c>
       <c r="C255">
-        <v>4311499000</v>
+        <v>4318985000</v>
       </c>
       <c r="D255" t="s">
         <v>444</v>
       </c>
       <c r="E255">
-        <v>4311499</v>
+        <v>4318985</v>
       </c>
       <c r="F255" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="I255" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>4322024000</v>
+      </c>
+      <c r="B256">
+        <v>4322024000</v>
+      </c>
+      <c r="C256">
+        <v>4322024000</v>
+      </c>
+      <c r="D256" t="s">
         <v>445</v>
       </c>
-      <c r="H255" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="256" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A256">
-        <v>4318985000</v>
-      </c>
-      <c r="B256">
-        <v>378416000</v>
-      </c>
-      <c r="C256">
-        <v>4318985000</v>
-      </c>
-      <c r="D256" t="s">
+      <c r="E256">
+        <v>4322024</v>
+      </c>
+      <c r="F256" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="E256">
-        <v>4318985</v>
-      </c>
-      <c r="F256" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="I256" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="257" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="H256" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A257">
-        <v>4322024000</v>
+        <v>4344489000</v>
       </c>
       <c r="B257">
-        <v>4322024000</v>
+        <v>4137275000</v>
       </c>
       <c r="C257">
-        <v>4322024000</v>
+        <v>4344489000</v>
       </c>
       <c r="D257" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E257">
-        <v>4322024</v>
+        <v>4344489</v>
       </c>
       <c r="F257" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H257" t="s">
-        <v>449</v>
+        <v>501</v>
+      </c>
+      <c r="I257" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="258" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A258">
-        <v>4344489000</v>
+        <v>36712702000</v>
       </c>
       <c r="B258">
-        <v>4137275000</v>
+        <v>36712702000</v>
       </c>
       <c r="C258">
-        <v>4344489000</v>
+        <v>36712702000</v>
       </c>
       <c r="D258" t="s">
+        <v>449</v>
+      </c>
+      <c r="E258">
+        <v>36712702</v>
+      </c>
+      <c r="F258" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="E258">
-        <v>4344489</v>
-      </c>
-      <c r="F258" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="I258" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="259" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="259" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A259">
-        <v>36712702000</v>
+        <v>37311061000</v>
       </c>
       <c r="B259">
-        <v>36712702000</v>
+        <v>37311061000</v>
       </c>
       <c r="C259">
-        <v>36712702000</v>
+        <v>37311061000</v>
       </c>
       <c r="D259" t="s">
         <v>451</v>
       </c>
       <c r="E259">
-        <v>36712702</v>
+        <v>37311061</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A260">
-        <v>37311061000</v>
+        <v>40479589000</v>
       </c>
       <c r="B260">
-        <v>37311061000</v>
+        <v>321319000</v>
       </c>
       <c r="C260">
-        <v>37311061000</v>
+        <v>40479589000</v>
       </c>
       <c r="D260" t="s">
         <v>453</v>
       </c>
       <c r="E260">
-        <v>37311061</v>
+        <v>40479589</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="261" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="I260" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A261">
-        <v>40479589000</v>
+        <v>40481901000</v>
       </c>
       <c r="B261">
-        <v>321319000</v>
+        <v>432571000</v>
       </c>
       <c r="C261">
-        <v>40479589000</v>
+        <v>40481901000</v>
       </c>
       <c r="D261" t="s">
         <v>455</v>
       </c>
       <c r="E261">
-        <v>40479589</v>
+        <v>40481901</v>
       </c>
       <c r="F261" s="1" t="s">
-        <v>456</v>
+        <v>513</v>
       </c>
       <c r="I261" t="s">
         <v>22</v>
@@ -8277,236 +8274,213 @@
     </row>
     <row r="262" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A262">
-        <v>40481901000</v>
+        <v>40481902000</v>
       </c>
       <c r="B262">
+        <v>40481902000</v>
+      </c>
+      <c r="C262">
+        <v>40481902000</v>
+      </c>
+      <c r="D262" t="s">
+        <v>456</v>
+      </c>
+      <c r="E262">
+        <v>40481902</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="H262" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>40490918000</v>
+      </c>
+      <c r="B263">
         <v>432571000</v>
       </c>
-      <c r="C262">
-        <v>40481901000</v>
-      </c>
-      <c r="D262" t="s">
-        <v>457</v>
-      </c>
-      <c r="E262">
-        <v>40481901</v>
-      </c>
-      <c r="F262" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="I262" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="263" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A263">
-        <v>40481902000</v>
-      </c>
-      <c r="B263">
-        <v>40481902000</v>
-      </c>
       <c r="C263">
-        <v>40481902000</v>
+        <v>40490918000</v>
       </c>
       <c r="D263" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E263">
-        <v>40481902</v>
+        <v>40490918</v>
       </c>
       <c r="F263" s="1" t="s">
-        <v>459</v>
+        <v>514</v>
       </c>
       <c r="H263" t="s">
-        <v>460</v>
+        <v>24</v>
+      </c>
+      <c r="I263" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="264" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A264">
-        <v>40490918000</v>
+        <v>42535714000</v>
       </c>
       <c r="B264">
-        <v>432571000</v>
+        <v>4137275000</v>
       </c>
       <c r="C264">
-        <v>40490918000</v>
+        <v>42535714000</v>
       </c>
       <c r="D264" t="s">
+        <v>460</v>
+      </c>
+      <c r="E264">
+        <v>42535714</v>
+      </c>
+      <c r="F264" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="E264">
-        <v>40490918</v>
-      </c>
-      <c r="F264" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="H264" t="s">
-        <v>24</v>
-      </c>
       <c r="I264" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="265" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A265">
-        <v>42535714000</v>
+        <v>43021132000</v>
       </c>
       <c r="B265">
-        <v>4137275000</v>
+        <v>43021132000</v>
       </c>
       <c r="C265">
-        <v>42535714000</v>
+        <v>43021132000</v>
       </c>
       <c r="D265" t="s">
         <v>462</v>
       </c>
       <c r="E265">
-        <v>42535714</v>
+        <v>43021132</v>
       </c>
       <c r="F265" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="I265" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="266" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266">
-        <v>43021132000</v>
+        <v>43021226000</v>
       </c>
       <c r="B266">
-        <v>43021132000</v>
+        <v>43021226000</v>
       </c>
       <c r="C266">
-        <v>43021132000</v>
+        <v>43021226000</v>
       </c>
       <c r="D266" t="s">
+        <v>550</v>
+      </c>
+      <c r="E266">
+        <v>43021226</v>
+      </c>
+      <c r="F266" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H266" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>43530714000</v>
+      </c>
+      <c r="B267">
+        <v>4094294000</v>
+      </c>
+      <c r="C267">
+        <v>43530714000</v>
+      </c>
+      <c r="D267" t="s">
         <v>464</v>
       </c>
-      <c r="E266">
-        <v>43021132</v>
-      </c>
-      <c r="F266" s="1" t="s">
+      <c r="E267">
+        <v>43530714</v>
+      </c>
+      <c r="F267" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="I267" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>44784217000</v>
+      </c>
+      <c r="B268">
+        <v>44784217000</v>
+      </c>
+      <c r="C268">
+        <v>44784217000</v>
+      </c>
+      <c r="D268" s="3" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A267">
-        <v>43021226000</v>
-      </c>
-      <c r="B267">
-        <v>43021226000</v>
-      </c>
-      <c r="C267">
-        <v>43021226000</v>
-      </c>
-      <c r="D267" t="s">
-        <v>552</v>
-      </c>
-      <c r="E267">
-        <v>43021226</v>
-      </c>
-      <c r="F267" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="H267" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="268" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A268">
-        <v>43530714000</v>
-      </c>
-      <c r="B268">
-        <v>4094294000</v>
-      </c>
-      <c r="C268">
-        <v>43530714000</v>
-      </c>
-      <c r="D268" t="s">
+      <c r="E268">
+        <v>44784217</v>
+      </c>
+      <c r="F268" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="E268">
-        <v>43530714</v>
-      </c>
-      <c r="F268" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="I268" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="269" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="H268" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>44784217000</v>
+        <v>45763653000</v>
       </c>
       <c r="B269">
-        <v>44784217000</v>
+        <v>45763653000</v>
       </c>
       <c r="C269">
-        <v>44784217000</v>
-      </c>
-      <c r="D269" s="3" t="s">
-        <v>467</v>
+        <v>45763653000</v>
+      </c>
+      <c r="D269" t="s">
+        <v>468</v>
       </c>
       <c r="E269">
-        <v>44784217</v>
+        <v>45763653</v>
       </c>
       <c r="F269" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="H269" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="270" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A270">
-        <v>45763653000</v>
+        <v>46271022000</v>
       </c>
       <c r="B270">
-        <v>45763653000</v>
+        <v>4030518000</v>
       </c>
       <c r="C270">
-        <v>45763653000</v>
+        <v>46271022000</v>
       </c>
       <c r="D270" t="s">
         <v>470</v>
       </c>
       <c r="E270">
-        <v>45763653</v>
+        <v>46271022</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="H270" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="271" spans="1:9" ht="270" x14ac:dyDescent="0.25">
-      <c r="A271">
-        <v>46271022000</v>
-      </c>
-      <c r="B271">
-        <v>4030518000</v>
-      </c>
-      <c r="C271">
-        <v>46271022000</v>
-      </c>
-      <c r="D271" t="s">
-        <v>472</v>
-      </c>
-      <c r="E271">
-        <v>46271022</v>
-      </c>
-      <c r="F271" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="I271" t="s">
+      <c r="I270" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I271">
+  <autoFilter ref="A1:I270">
     <sortState ref="A2:I271">
       <sortCondition ref="C1:C271"/>
     </sortState>

</xml_diff>

<commit_message>
Revert "removed 440703000,Trigeminal nerve disorder as no cohorts"
This reverts commit 9989459e6c63b503d3defd4cc6e8f6e64a2725d9.
</commit_message>
<xml_diff>
--- a/extras/PhenotypeDescription.xlsx
+++ b/extras/PhenotypeDescription.xlsx
@@ -15,14 +15,14 @@
     <sheet name="PhenotypeDescription" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PhenotypeDescription!$A$1:$I$270</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PhenotypeDescription!$A$1:$I$271</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="566">
   <si>
     <t>oldPhenotypeId</t>
   </si>
@@ -907,6 +907,12 @@
   </si>
   <si>
     <t>Overview: Pain and inflammation occur when too much uric acid crystallizes and deposits in the joints. Form of arthritis. Gout occurs when urate crystals accumulate in your joint, causing the inflammation and intense pain of a gout attackPresentation: Sudden, severe attacks of pain, swelling, redness and tenderness in the joints, often the joint at the base of the big toe. Symptoms come and go. Tophi - large, visible bumps made of urate crystals. Assessment: joint fluid test (from the affected joint), blood levels of uric acid and creatinine, xray, ultrasound, sual energy CT scan Plan: NSAIDs, Colchicine, Corticosteroids; xanthine oxidase inhibitors (XOIs) and uricosurics to prevent gout complications Prognosis: Early gout diagnosis, therapy enables most patients to live a normal life. Gout is a highly treatable form of arthritis.</t>
+  </si>
+  <si>
+    <t>Trigeminal nerve disorder</t>
+  </si>
+  <si>
+    <t>Overview: Trigeminal (fifth) nerve, largest of the cranial nerve - supplies sensation to the skin of the face and anterior half of head. Motor component - muscles of mastication and tensor tympani of middle ear hearing. Most commonly disorder is Trigeminal neuralgia (tic douloureux) TN - mainly due to compression of the trigeminal nerve root, demyelination (multiple sclerosis). Trigemenial nerve disorder may also present without pain, e.g. trigeminal neuropathy with sensory loss on the face, with weakness of muscles of masticatio- deviation of jaw on opening. Presentation: TN is characterized by recurrent brief episodes of excruciating unilateral electric shock like pain in the lips, gums, cheek or chin. TN is mosstly clustered among middle-aged and elderly persons are affected, with ~ 60% in women. Assessment: TN is a clinical diagnosis - but detailed investigation using neuroimaging to identify cause. Rule out herpes zoster, post traumatic.  Plan: carbamazepine or oxcarbazepine is first line. Gabapentin for non responders. Lidocaine, phenytoin for rescue therapy. Occassionally surgery (gamma knife radiosurgery, rhizotomy, microvascular decompression). Prognosis: highly variable, may go into months of remission. recurrence is common.</t>
   </si>
   <si>
     <t>Takayasu's disease</t>
@@ -2556,11 +2562,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I270"/>
+  <dimension ref="A1:I271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A167" sqref="A167:XFD167"/>
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,7 +2627,7 @@
         <v>24134</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
@@ -2664,7 +2670,7 @@
         <v>27918</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
@@ -2687,7 +2693,7 @@
         <v>30753</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
@@ -2710,7 +2716,7 @@
         <v>31317</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -2733,7 +2739,7 @@
         <v>31967</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="I7" t="s">
         <v>22</v>
@@ -2779,7 +2785,7 @@
         <v>287</v>
       </c>
       <c r="H9" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2799,7 +2805,7 @@
         <v>75860</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="I10" t="s">
         <v>22</v>
@@ -2845,7 +2851,7 @@
         <v>77074</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H12" t="s">
         <v>24</v>
@@ -2894,7 +2900,7 @@
         <v>80182</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -2977,7 +2983,7 @@
         <v>81893</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="I18" t="s">
         <v>22</v>
@@ -3000,7 +3006,7 @@
         <v>81902</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -3083,7 +3089,7 @@
         <v>132797</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="I23" t="s">
         <v>22</v>
@@ -3106,7 +3112,7 @@
         <v>133169</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="I24" t="s">
         <v>22</v>
@@ -3212,7 +3218,7 @@
         <v>137977</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="I29" t="s">
         <v>22</v>
@@ -3275,7 +3281,7 @@
         <v>138994</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="I32" t="s">
         <v>22</v>
@@ -3361,7 +3367,7 @@
         <v>140352</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="I36" t="s">
         <v>22</v>
@@ -3464,7 +3470,7 @@
         <v>192359</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="I41" t="s">
         <v>22</v>
@@ -3550,7 +3556,7 @@
         <v>194133</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="I45" t="s">
         <v>22</v>
@@ -3593,7 +3599,7 @@
         <v>194992</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="I47" t="s">
         <v>22</v>
@@ -3616,7 +3622,7 @@
         <v>196523</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="I48" t="s">
         <v>22</v>
@@ -3791,7 +3797,7 @@
         <v>200219</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="I56" t="s">
         <v>22</v>
@@ -3863,7 +3869,7 @@
         <v>201254</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="I59" t="s">
         <v>22</v>
@@ -3886,7 +3892,7 @@
         <v>201340</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="I60" t="s">
         <v>22</v>
@@ -3909,7 +3915,7 @@
         <v>201606</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="I61" t="s">
         <v>22</v>
@@ -3943,7 +3949,7 @@
         <v>201820000</v>
       </c>
       <c r="D63" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="E63">
         <v>201820</v>
@@ -3952,7 +3958,7 @@
         <v>287</v>
       </c>
       <c r="H63" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -3972,7 +3978,7 @@
         <v>201826</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="I64" t="s">
         <v>22</v>
@@ -4038,7 +4044,7 @@
         <v>254761</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="I67" t="s">
         <v>22</v>
@@ -4144,7 +4150,7 @@
         <v>312327</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I72" t="s">
         <v>22</v>
@@ -4167,7 +4173,7 @@
         <v>312437</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="I73" t="s">
         <v>22</v>
@@ -4210,7 +4216,7 @@
         <v>313217</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="I75" t="s">
         <v>22</v>
@@ -4233,7 +4239,7 @@
         <v>313223</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="I76" t="s">
         <v>22</v>
@@ -4256,7 +4262,7 @@
         <v>313459</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="210" x14ac:dyDescent="0.25">
@@ -4319,7 +4325,7 @@
         <v>314383</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="I80" t="s">
         <v>22</v>
@@ -4388,7 +4394,7 @@
         <v>317009</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="I83" t="s">
         <v>22</v>
@@ -4411,7 +4417,7 @@
         <v>317576</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="I84" t="s">
         <v>22</v>
@@ -4566,7 +4572,7 @@
         <v>321042</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="H91" t="s">
         <v>24</v>
@@ -4615,7 +4621,7 @@
         <v>321318</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="I93" t="s">
         <v>22</v>
@@ -4658,7 +4664,7 @@
         <v>321588</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="H95" t="s">
         <v>24</v>
@@ -4704,7 +4710,7 @@
         <v>373503</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="I97" t="s">
         <v>22</v>
@@ -4753,7 +4759,7 @@
         <v>374028</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="I99" t="s">
         <v>22</v>
@@ -4796,7 +4802,7 @@
         <v>374377</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="H101" t="s">
         <v>24</v>
@@ -5000,7 +5006,7 @@
         <v>378253</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="I110" t="s">
         <v>22</v>
@@ -5023,7 +5029,7 @@
         <v>378414</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="I111" t="s">
         <v>22</v>
@@ -5086,7 +5092,7 @@
         <v>380378</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="I114" t="s">
         <v>22</v>
@@ -5212,7 +5218,7 @@
         <v>432571000</v>
       </c>
       <c r="D120" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E120">
         <v>432571000</v>
@@ -5261,7 +5267,7 @@
         <v>432595</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5324,7 +5330,7 @@
         <v>432870</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="I125" t="s">
         <v>22</v>
@@ -5393,7 +5399,7 @@
         <v>433595</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="I128" t="s">
         <v>22</v>
@@ -5496,7 +5502,7 @@
         <v>434592</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="I133" t="s">
         <v>22</v>
@@ -5651,7 +5657,7 @@
         <v>248</v>
       </c>
       <c r="H140" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5671,7 +5677,7 @@
         <v>436096</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="I141" t="s">
         <v>22</v>
@@ -5714,7 +5720,7 @@
         <v>4307095</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="I143" t="s">
         <v>22</v>
@@ -5800,7 +5806,7 @@
         <v>436962</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="I147" t="s">
         <v>22</v>
@@ -5823,7 +5829,7 @@
         <v>437082</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="I148" t="s">
         <v>22</v>
@@ -5889,7 +5895,7 @@
         <v>437312</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="I151" t="s">
         <v>22</v>
@@ -5932,7 +5938,7 @@
         <v>437663</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="H153" t="s">
         <v>269</v>
@@ -6072,7 +6078,7 @@
         <v>439776000</v>
       </c>
       <c r="D160" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E160">
         <v>439776</v>
@@ -6144,7 +6150,7 @@
         <v>440377</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="H163" t="s">
         <v>24</v>
@@ -6215,62 +6221,62 @@
     </row>
     <row r="167" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>440740000</v>
+        <v>440703000</v>
       </c>
       <c r="B167">
-        <v>4137275000</v>
+        <v>440703000</v>
       </c>
       <c r="C167">
-        <v>440740000</v>
+        <v>440703000</v>
       </c>
       <c r="D167" t="s">
         <v>295</v>
       </c>
       <c r="E167">
-        <v>440740</v>
+        <v>440703</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="I167" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>440925000</v>
+        <v>440740000</v>
       </c>
       <c r="B168">
-        <v>440925000</v>
+        <v>4137275000</v>
       </c>
       <c r="C168">
-        <v>440925000</v>
+        <v>440740000</v>
       </c>
       <c r="D168" t="s">
         <v>297</v>
       </c>
       <c r="E168">
-        <v>440925</v>
+        <v>440740</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="I168" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>440940000</v>
+        <v>440925000</v>
       </c>
       <c r="B169">
-        <v>440940000</v>
+        <v>440925000</v>
       </c>
       <c r="C169">
-        <v>440940000</v>
+        <v>440925000</v>
       </c>
       <c r="D169" t="s">
         <v>299</v>
       </c>
       <c r="E169">
-        <v>440940</v>
+        <v>440925</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>300</v>
@@ -6278,154 +6284,151 @@
     </row>
     <row r="170" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>441202000</v>
+        <v>440940000</v>
       </c>
       <c r="B170">
-        <v>43021226000</v>
+        <v>440940000</v>
       </c>
       <c r="C170">
-        <v>441202000</v>
-      </c>
-      <c r="D170" s="2" t="s">
+        <v>440940000</v>
+      </c>
+      <c r="D170" t="s">
         <v>301</v>
       </c>
       <c r="E170">
-        <v>441202</v>
+        <v>440940</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="I170" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>441284000</v>
+        <v>441202000</v>
       </c>
       <c r="B171">
-        <v>441284000</v>
+        <v>43021226000</v>
       </c>
       <c r="C171">
-        <v>441284000</v>
-      </c>
-      <c r="D171" t="s">
+        <v>441202000</v>
+      </c>
+      <c r="D171" s="2" t="s">
         <v>303</v>
       </c>
       <c r="E171">
-        <v>441284</v>
+        <v>441202</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="I171" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>441408000</v>
+        <v>441284000</v>
       </c>
       <c r="B172">
-        <v>4094294000</v>
+        <v>441284000</v>
       </c>
       <c r="C172">
-        <v>441408000</v>
+        <v>441284000</v>
       </c>
       <c r="D172" t="s">
         <v>305</v>
       </c>
       <c r="E172">
-        <v>441408</v>
+        <v>441284</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="I172" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>441542000</v>
+        <v>441408000</v>
       </c>
       <c r="B173">
         <v>4094294000</v>
       </c>
       <c r="C173">
+        <v>441408000</v>
+      </c>
+      <c r="D173" t="s">
+        <v>307</v>
+      </c>
+      <c r="E173">
+        <v>441408</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="I173" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A174">
         <v>441542000</v>
       </c>
-      <c r="D173" t="s">
-        <v>306</v>
-      </c>
-      <c r="E173">
+      <c r="B174">
+        <v>4094294000</v>
+      </c>
+      <c r="C174">
+        <v>441542000</v>
+      </c>
+      <c r="D174" t="s">
+        <v>308</v>
+      </c>
+      <c r="E174">
         <v>441542</v>
       </c>
-      <c r="F173" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="I173" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A174">
+      <c r="F174" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="I174" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A175">
         <v>441788000</v>
       </c>
-      <c r="B174">
+      <c r="B175">
         <v>441788000</v>
       </c>
-      <c r="C174">
+      <c r="C175">
         <v>441788000</v>
-      </c>
-      <c r="D174" t="s">
-        <v>307</v>
-      </c>
-      <c r="E174">
-        <v>441788</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A175">
-        <v>441848000</v>
-      </c>
-      <c r="B175">
-        <v>0</v>
-      </c>
-      <c r="C175">
-        <v>441848000</v>
       </c>
       <c r="D175" t="s">
         <v>309</v>
       </c>
       <c r="E175">
-        <v>441848</v>
+        <v>441788</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="I175" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>442752000</v>
+        <v>441848000</v>
       </c>
       <c r="B176">
-        <v>4094294000</v>
+        <v>0</v>
       </c>
       <c r="C176">
-        <v>442752000</v>
+        <v>441848000</v>
       </c>
       <c r="D176" t="s">
         <v>311</v>
       </c>
       <c r="E176">
-        <v>442752</v>
+        <v>441848</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>543</v>
+        <v>312</v>
       </c>
       <c r="I176" t="s">
         <v>22</v>
@@ -6433,39 +6436,42 @@
     </row>
     <row r="177" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A177">
+        <v>442752000</v>
+      </c>
+      <c r="B177">
+        <v>4094294000</v>
+      </c>
+      <c r="C177">
+        <v>442752000</v>
+      </c>
+      <c r="D177" t="s">
+        <v>313</v>
+      </c>
+      <c r="E177">
+        <v>442752</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="I177" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A178">
         <v>443213000</v>
       </c>
-      <c r="B177">
+      <c r="B178">
         <v>443213000</v>
       </c>
-      <c r="C177">
+      <c r="C178">
         <v>443213000</v>
-      </c>
-      <c r="D177" t="s">
-        <v>312</v>
-      </c>
-      <c r="E177">
-        <v>443213</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A178">
-        <v>443387000</v>
-      </c>
-      <c r="B178">
-        <v>443387000</v>
-      </c>
-      <c r="C178">
-        <v>443387000</v>
       </c>
       <c r="D178" t="s">
         <v>314</v>
       </c>
       <c r="E178">
-        <v>443387</v>
+        <v>443213</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>315</v>
@@ -6473,696 +6479,693 @@
     </row>
     <row r="179" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>443392000</v>
+        <v>443387000</v>
       </c>
       <c r="B179">
-        <v>443392000</v>
+        <v>443387000</v>
       </c>
       <c r="C179">
-        <v>443392000</v>
-      </c>
-      <c r="D179" s="3" t="s">
+        <v>443387000</v>
+      </c>
+      <c r="D179" t="s">
         <v>316</v>
       </c>
       <c r="E179">
-        <v>443392</v>
+        <v>443387</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>443454000</v>
+        <v>443392000</v>
       </c>
       <c r="B180">
-        <v>381591000</v>
+        <v>443392000</v>
       </c>
       <c r="C180">
-        <v>443454000</v>
-      </c>
-      <c r="D180" t="s">
+        <v>443392000</v>
+      </c>
+      <c r="D180" s="3" t="s">
         <v>318</v>
       </c>
       <c r="E180">
-        <v>443454</v>
+        <v>443392</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="I180" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>443700000</v>
+        <v>443454000</v>
       </c>
       <c r="B181">
-        <v>443700000</v>
+        <v>381591000</v>
       </c>
       <c r="C181">
-        <v>443700000</v>
+        <v>443454000</v>
       </c>
       <c r="D181" t="s">
         <v>320</v>
       </c>
       <c r="E181">
-        <v>443700</v>
+        <v>443454</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I181" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A182">
+        <v>443700000</v>
+      </c>
+      <c r="B182">
+        <v>443700000</v>
+      </c>
+      <c r="C182">
+        <v>443700000</v>
+      </c>
+      <c r="D182" t="s">
+        <v>322</v>
+      </c>
+      <c r="E182">
+        <v>443700</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183">
         <v>443723000</v>
       </c>
-      <c r="B182">
+      <c r="B183">
         <v>443723000</v>
       </c>
-      <c r="C182">
+      <c r="C183">
         <v>443723000</v>
       </c>
-      <c r="D182" t="s">
-        <v>557</v>
-      </c>
-      <c r="E182">
+      <c r="D183" t="s">
+        <v>559</v>
+      </c>
+      <c r="E183">
         <v>443723</v>
       </c>
-      <c r="F182" s="1" t="s">
+      <c r="F183" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A183">
+    <row r="184" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A184">
         <v>443727000</v>
       </c>
-      <c r="B183">
+      <c r="B184">
         <v>201820000</v>
       </c>
-      <c r="C183">
+      <c r="C184">
         <v>443727000</v>
       </c>
-      <c r="D183" t="s">
-        <v>322</v>
-      </c>
-      <c r="E183">
+      <c r="D184" t="s">
+        <v>324</v>
+      </c>
+      <c r="E184">
         <v>443727</v>
       </c>
-      <c r="F183" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="I183" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A184">
+      <c r="F184" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="I184" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A185">
         <v>444044000</v>
       </c>
-      <c r="B184">
+      <c r="B185">
         <v>4030518000</v>
       </c>
-      <c r="C184">
+      <c r="C185">
         <v>444044000</v>
       </c>
-      <c r="D184" t="s">
-        <v>323</v>
-      </c>
-      <c r="E184">
+      <c r="D185" t="s">
+        <v>325</v>
+      </c>
+      <c r="E185">
         <v>444044</v>
       </c>
-      <c r="F184" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="I184" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A185">
+      <c r="F185" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="I185" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A186">
         <v>444070000</v>
       </c>
-      <c r="B185">
+      <c r="B186">
         <v>4094294000</v>
       </c>
-      <c r="C185">
+      <c r="C186">
         <v>444070000</v>
       </c>
-      <c r="D185" t="s">
-        <v>324</v>
-      </c>
-      <c r="E185">
+      <c r="D186" t="s">
+        <v>326</v>
+      </c>
+      <c r="E186">
         <v>444070</v>
       </c>
-      <c r="F185" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="I185" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A186">
+      <c r="F186" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="I186" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A187">
         <v>444247000</v>
       </c>
-      <c r="B186">
+      <c r="B187">
         <v>444247000</v>
       </c>
-      <c r="C186">
+      <c r="C187">
         <v>444247000</v>
-      </c>
-      <c r="D186" t="s">
-        <v>325</v>
-      </c>
-      <c r="E186">
-        <v>444247</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A187">
-        <v>444429000</v>
-      </c>
-      <c r="B187">
-        <v>444429000</v>
-      </c>
-      <c r="C187">
-        <v>444429000</v>
       </c>
       <c r="D187" t="s">
         <v>327</v>
       </c>
       <c r="E187">
-        <v>444429</v>
+        <v>444247</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>4000634000</v>
+        <v>444429000</v>
       </c>
       <c r="B188">
-        <v>73553000</v>
+        <v>444429000</v>
       </c>
       <c r="C188">
-        <v>4000634000</v>
+        <v>444429000</v>
       </c>
       <c r="D188" t="s">
         <v>329</v>
       </c>
       <c r="E188">
-        <v>4000634</v>
+        <v>444429</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="H188" t="s">
+    </row>
+    <row r="189" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>4000634000</v>
+      </c>
+      <c r="B189">
+        <v>73553000</v>
+      </c>
+      <c r="C189">
+        <v>4000634000</v>
+      </c>
+      <c r="D189" t="s">
         <v>331</v>
       </c>
-      <c r="I188" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A189">
+      <c r="E189">
+        <v>4000634</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="H189" t="s">
+        <v>333</v>
+      </c>
+      <c r="I189" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A190">
         <v>4002359000</v>
       </c>
-      <c r="B189">
+      <c r="B190">
         <v>436081000</v>
       </c>
-      <c r="C189">
+      <c r="C190">
         <v>4002359000</v>
-      </c>
-      <c r="D189" t="s">
-        <v>332</v>
-      </c>
-      <c r="E189">
-        <v>4002359</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="I189" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A190">
-        <v>4013643000</v>
-      </c>
-      <c r="B190">
-        <v>4013643000</v>
-      </c>
-      <c r="C190">
-        <v>4013643000</v>
       </c>
       <c r="D190" t="s">
         <v>334</v>
       </c>
       <c r="E190">
-        <v>4013643</v>
+        <v>4002359</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I190" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>4024659000</v>
+        <v>4013643000</v>
       </c>
       <c r="B191">
-        <v>201820000</v>
+        <v>4013643000</v>
       </c>
       <c r="C191">
-        <v>4024659000</v>
+        <v>4013643000</v>
       </c>
       <c r="D191" t="s">
         <v>336</v>
       </c>
       <c r="E191">
-        <v>4024659</v>
+        <v>4013643</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="H191" t="s">
         <v>337</v>
       </c>
-      <c r="I191" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>4027537000</v>
+        <v>4024659000</v>
       </c>
       <c r="B192">
-        <v>4027537000</v>
+        <v>201820000</v>
       </c>
       <c r="C192">
-        <v>4027537000</v>
+        <v>4024659000</v>
       </c>
       <c r="D192" t="s">
         <v>338</v>
       </c>
       <c r="E192">
+        <v>4024659</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="H192" t="s">
+        <v>339</v>
+      </c>
+      <c r="I192" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>4027537000</v>
+      </c>
+      <c r="B193">
+        <v>4027537000</v>
+      </c>
+      <c r="C193">
+        <v>4027537000</v>
+      </c>
+      <c r="D193" t="s">
+        <v>340</v>
+      </c>
+      <c r="E193">
         <v>4027537</v>
       </c>
-      <c r="F192" s="1" t="s">
+      <c r="F193" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A193">
+    <row r="194" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A194">
         <v>4028363000</v>
       </c>
-      <c r="B193">
+      <c r="B194">
         <v>4028363000</v>
       </c>
-      <c r="C193">
+      <c r="C194">
         <v>4028363000</v>
-      </c>
-      <c r="D193" t="s">
-        <v>339</v>
-      </c>
-      <c r="E193">
-        <v>4028363</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" ht="375" x14ac:dyDescent="0.25">
-      <c r="A194">
-        <v>4030518000</v>
-      </c>
-      <c r="B194">
-        <v>4030518000</v>
-      </c>
-      <c r="C194">
-        <v>4030518000</v>
       </c>
       <c r="D194" t="s">
         <v>341</v>
       </c>
       <c r="E194">
-        <v>4030518</v>
+        <v>4028363</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" ht="375" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>4038838000</v>
+        <v>4030518000</v>
       </c>
       <c r="B195">
-        <v>432571000</v>
+        <v>4030518000</v>
       </c>
       <c r="C195">
-        <v>4038838000</v>
+        <v>4030518000</v>
       </c>
       <c r="D195" t="s">
         <v>343</v>
       </c>
       <c r="E195">
+        <v>4030518</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>4038838000</v>
+      </c>
+      <c r="B196">
+        <v>432571000</v>
+      </c>
+      <c r="C196">
+        <v>4038838000</v>
+      </c>
+      <c r="D196" t="s">
+        <v>345</v>
+      </c>
+      <c r="E196">
         <v>4038838</v>
       </c>
-      <c r="F195" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="I195" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B196">
+      <c r="F196" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="I196" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B197">
         <v>4043371000</v>
       </c>
-      <c r="C196">
+      <c r="C197">
         <v>4043371000</v>
       </c>
-      <c r="D196" t="s">
-        <v>472</v>
-      </c>
-      <c r="E196">
+      <c r="D197" t="s">
+        <v>474</v>
+      </c>
+      <c r="E197">
         <v>4043371</v>
       </c>
-      <c r="F196" s="1" t="s">
+      <c r="F197" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="H196" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A197">
+      <c r="H197" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A198">
         <v>4046338000</v>
       </c>
-      <c r="B197">
+      <c r="B198">
         <v>4046338000</v>
       </c>
-      <c r="C197">
+      <c r="C198">
         <v>4046338000</v>
-      </c>
-      <c r="D197" t="s">
-        <v>344</v>
-      </c>
-      <c r="E197">
-        <v>4046338</v>
-      </c>
-      <c r="F197" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A198">
-        <v>4058821000</v>
-      </c>
-      <c r="B198">
-        <v>4212540000</v>
-      </c>
-      <c r="C198">
-        <v>4058821000</v>
       </c>
       <c r="D198" t="s">
         <v>346</v>
       </c>
       <c r="E198">
-        <v>4058821</v>
+        <v>4046338</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="I198" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A199">
+        <v>4058821000</v>
+      </c>
+      <c r="B199">
+        <v>4212540000</v>
+      </c>
+      <c r="C199">
+        <v>4058821000</v>
+      </c>
+      <c r="D199" t="s">
+        <v>348</v>
+      </c>
+      <c r="E199">
+        <v>4058821</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="I199" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A200">
         <v>4063434000</v>
       </c>
-      <c r="B199">
+      <c r="B200">
         <v>140168000</v>
       </c>
-      <c r="C199">
+      <c r="C200">
         <v>4063434000</v>
       </c>
-      <c r="D199" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="E199">
+      <c r="D200" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E200">
         <v>4063434</v>
       </c>
-      <c r="F199" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="I199" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A200">
+      <c r="F200" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I200" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A201">
         <v>4064161000</v>
       </c>
-      <c r="B200">
+      <c r="B201">
         <v>4212540000</v>
       </c>
-      <c r="C200">
+      <c r="C201">
         <v>4064161000</v>
-      </c>
-      <c r="D200" t="s">
-        <v>349</v>
-      </c>
-      <c r="E200">
-        <v>4064161</v>
-      </c>
-      <c r="F200" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="I200" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A201">
-        <v>4067106000</v>
-      </c>
-      <c r="B201">
-        <v>4067106000</v>
-      </c>
-      <c r="C201">
-        <v>4067106000</v>
       </c>
       <c r="D201" t="s">
         <v>351</v>
       </c>
       <c r="E201">
-        <v>4067106</v>
+        <v>4064161</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="I201" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>4070552000</v>
+        <v>4067106000</v>
       </c>
       <c r="B202">
-        <v>4164770000</v>
+        <v>4067106000</v>
       </c>
       <c r="C202">
-        <v>4070552000</v>
+        <v>4067106000</v>
       </c>
       <c r="D202" t="s">
         <v>353</v>
       </c>
       <c r="E202">
-        <v>4070552</v>
+        <v>4067106</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="H202" t="s">
+    </row>
+    <row r="203" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>4070552000</v>
+      </c>
+      <c r="B203">
+        <v>4164770000</v>
+      </c>
+      <c r="C203">
+        <v>4070552000</v>
+      </c>
+      <c r="D203" t="s">
         <v>355</v>
       </c>
-      <c r="I202" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="203" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A203">
+      <c r="E203">
+        <v>4070552</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="H203" t="s">
+        <v>357</v>
+      </c>
+      <c r="I203" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A204">
         <v>4074815000</v>
       </c>
-      <c r="B203">
+      <c r="B204">
         <v>4043371000</v>
       </c>
-      <c r="C203">
+      <c r="C204">
         <v>4074815000</v>
       </c>
-      <c r="D203" t="s">
-        <v>356</v>
-      </c>
-      <c r="E203">
+      <c r="D204" t="s">
+        <v>358</v>
+      </c>
+      <c r="E204">
         <v>4074815</v>
       </c>
-      <c r="F203" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="I203" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A204">
+      <c r="F204" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="I204" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A205">
         <v>4079843000</v>
       </c>
-      <c r="B204">
+      <c r="B205">
         <v>4306655000</v>
       </c>
-      <c r="C204">
+      <c r="C205">
         <v>4079843000</v>
       </c>
-      <c r="D204" t="s">
-        <v>357</v>
-      </c>
-      <c r="E204">
+      <c r="D205" t="s">
+        <v>359</v>
+      </c>
+      <c r="E205">
         <v>4079843</v>
       </c>
-      <c r="F204" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="I204" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="205" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A205">
+      <c r="F205" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I205" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A206">
         <v>4091559000</v>
       </c>
-      <c r="B205">
+      <c r="B206">
         <v>378135000</v>
       </c>
-      <c r="C205">
+      <c r="C206">
         <v>4091559000</v>
-      </c>
-      <c r="D205" t="s">
-        <v>358</v>
-      </c>
-      <c r="E205">
-        <v>4091559</v>
-      </c>
-      <c r="F205" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="I205" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A206">
-        <v>4092289000</v>
-      </c>
-      <c r="B206">
-        <v>4092289000</v>
-      </c>
-      <c r="C206">
-        <v>4092289000</v>
       </c>
       <c r="D206" t="s">
         <v>360</v>
       </c>
       <c r="E206">
-        <v>4092289</v>
+        <v>4091559</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I206" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A207">
+        <v>4092289000</v>
+      </c>
+      <c r="B207">
+        <v>4092289000</v>
+      </c>
+      <c r="C207">
+        <v>4092289000</v>
+      </c>
+      <c r="D207" t="s">
+        <v>362</v>
+      </c>
+      <c r="E207">
+        <v>4092289</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208">
         <v>4094294000</v>
       </c>
-      <c r="B207">
+      <c r="B208">
         <v>4094294000</v>
       </c>
-      <c r="C207">
+      <c r="C208">
         <v>4094294000</v>
       </c>
-      <c r="D207" t="s">
-        <v>520</v>
-      </c>
-      <c r="E207">
+      <c r="D208" t="s">
+        <v>522</v>
+      </c>
+      <c r="E208">
         <v>4094294</v>
       </c>
-      <c r="F207" s="1" t="s">
+      <c r="F208" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A208">
+    <row r="209" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A209">
         <v>4098292000</v>
       </c>
-      <c r="B208">
+      <c r="B209">
         <v>4098292000</v>
       </c>
-      <c r="C208">
+      <c r="C209">
         <v>4098292000</v>
-      </c>
-      <c r="D208" t="s">
-        <v>362</v>
-      </c>
-      <c r="E208">
-        <v>4098292</v>
-      </c>
-      <c r="F208" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A209">
-        <v>4098597000</v>
-      </c>
-      <c r="B209">
-        <v>436081000</v>
-      </c>
-      <c r="C209">
-        <v>4098597000</v>
       </c>
       <c r="D209" t="s">
         <v>364</v>
       </c>
       <c r="E209">
-        <v>4098597</v>
+        <v>4098292</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="I209" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="210" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>4101602000</v>
+        <v>4098597000</v>
       </c>
       <c r="B210">
-        <v>4137275000</v>
+        <v>436081000</v>
       </c>
       <c r="C210">
-        <v>4101602000</v>
+        <v>4098597000</v>
       </c>
       <c r="D210" t="s">
         <v>366</v>
       </c>
       <c r="E210">
-        <v>4101602</v>
+        <v>4098597</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>367</v>
@@ -7171,861 +7174,864 @@
         <v>22</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>4103295000</v>
+        <v>4101602000</v>
       </c>
       <c r="B211">
-        <v>44784217000</v>
+        <v>4137275000</v>
       </c>
       <c r="C211">
-        <v>4103295000</v>
+        <v>4101602000</v>
       </c>
       <c r="D211" t="s">
         <v>368</v>
       </c>
       <c r="E211">
+        <v>4101602</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="I211" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>4103295000</v>
+      </c>
+      <c r="B212">
+        <v>44784217000</v>
+      </c>
+      <c r="C212">
+        <v>4103295000</v>
+      </c>
+      <c r="D212" t="s">
+        <v>370</v>
+      </c>
+      <c r="E212">
         <v>4103295</v>
       </c>
-      <c r="F211" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="I211" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="212" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A212">
+      <c r="F212" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="I212" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A213">
         <v>4112853000</v>
       </c>
-      <c r="B212">
+      <c r="B213">
         <v>4112853000</v>
       </c>
-      <c r="C212">
+      <c r="C213">
         <v>4112853000</v>
-      </c>
-      <c r="D212" t="s">
-        <v>369</v>
-      </c>
-      <c r="E212">
-        <v>4112853</v>
-      </c>
-      <c r="F212" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="213" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A213">
-        <v>4124836000</v>
-      </c>
-      <c r="B213">
-        <v>321052000</v>
-      </c>
-      <c r="C213">
-        <v>4124836000</v>
       </c>
       <c r="D213" t="s">
         <v>371</v>
       </c>
       <c r="E213">
-        <v>4124836</v>
+        <v>4112853</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="I213" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="214" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>4131909000</v>
+        <v>4124836000</v>
       </c>
       <c r="B214">
-        <v>4131909000</v>
+        <v>321052000</v>
       </c>
       <c r="C214">
-        <v>4131909000</v>
+        <v>4124836000</v>
       </c>
       <c r="D214" t="s">
         <v>373</v>
       </c>
       <c r="E214">
-        <v>4131909</v>
+        <v>4124836</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="215" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I214" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>4133004000</v>
+        <v>4131909000</v>
       </c>
       <c r="B215">
-        <v>4133004000</v>
+        <v>4131909000</v>
       </c>
       <c r="C215">
-        <v>4133004000</v>
+        <v>4131909000</v>
       </c>
       <c r="D215" t="s">
         <v>375</v>
       </c>
       <c r="E215">
-        <v>4133004</v>
+        <v>4131909</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>4137275000</v>
+        <v>4133004000</v>
       </c>
       <c r="B216">
-        <v>4137275000</v>
+        <v>4133004000</v>
       </c>
       <c r="C216">
-        <v>4137275000</v>
+        <v>4133004000</v>
       </c>
       <c r="D216" t="s">
         <v>377</v>
       </c>
       <c r="E216">
-        <v>4137275</v>
+        <v>4133004</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>4138837000</v>
+        <v>4137275000</v>
       </c>
       <c r="B217">
-        <v>4189294000</v>
+        <v>4137275000</v>
       </c>
       <c r="C217">
-        <v>4138837000</v>
+        <v>4137275000</v>
       </c>
       <c r="D217" t="s">
         <v>379</v>
       </c>
       <c r="E217">
-        <v>4138837</v>
+        <v>4137275</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="H217" t="s">
         <v>380</v>
       </c>
-      <c r="I217" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="218" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>4139034000</v>
+        <v>4138837000</v>
       </c>
       <c r="B218">
-        <v>4139034000</v>
+        <v>4189294000</v>
       </c>
       <c r="C218">
-        <v>4139034000</v>
+        <v>4138837000</v>
       </c>
       <c r="D218" t="s">
         <v>381</v>
       </c>
       <c r="E218">
-        <v>4139034</v>
+        <v>4138837</v>
       </c>
       <c r="F218" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="H218" t="s">
         <v>382</v>
       </c>
-      <c r="H218" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="219" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="I218" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>4147411000</v>
+        <v>4139034000</v>
       </c>
       <c r="B219">
-        <v>432571000</v>
+        <v>4139034000</v>
       </c>
       <c r="C219">
-        <v>4147411000</v>
+        <v>4139034000</v>
       </c>
       <c r="D219" t="s">
         <v>383</v>
       </c>
       <c r="E219">
+        <v>4139034</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="H219" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>4147411000</v>
+      </c>
+      <c r="B220">
+        <v>432571000</v>
+      </c>
+      <c r="C220">
+        <v>4147411000</v>
+      </c>
+      <c r="D220" t="s">
+        <v>385</v>
+      </c>
+      <c r="E220">
         <v>4147411</v>
       </c>
-      <c r="F219" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="I219" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="220" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A220">
+      <c r="F220" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="I220" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A221">
         <v>4163261000</v>
       </c>
-      <c r="B220">
+      <c r="B221">
         <v>4163261000</v>
       </c>
-      <c r="C220">
+      <c r="C221">
         <v>4163261000</v>
-      </c>
-      <c r="D220" t="s">
-        <v>384</v>
-      </c>
-      <c r="E220">
-        <v>4163261</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A221">
-        <v>4164770000</v>
-      </c>
-      <c r="B221">
-        <v>4164770000</v>
-      </c>
-      <c r="C221">
-        <v>4164770000</v>
       </c>
       <c r="D221" t="s">
         <v>386</v>
       </c>
       <c r="E221">
-        <v>4164770</v>
+        <v>4163261</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>4169095000</v>
+        <v>4164770000</v>
       </c>
       <c r="B222">
-        <v>4094294000</v>
+        <v>4164770000</v>
       </c>
       <c r="C222">
-        <v>4169095000</v>
+        <v>4164770000</v>
       </c>
       <c r="D222" t="s">
         <v>388</v>
       </c>
       <c r="E222">
+        <v>4164770</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>4169095000</v>
+      </c>
+      <c r="B223">
+        <v>4094294000</v>
+      </c>
+      <c r="C223">
+        <v>4169095000</v>
+      </c>
+      <c r="D223" t="s">
+        <v>390</v>
+      </c>
+      <c r="E223">
         <v>4169095</v>
       </c>
-      <c r="F222" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="I222" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="223" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A223">
+      <c r="F223" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="I223" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A224">
         <v>4174977000</v>
       </c>
-      <c r="B223">
+      <c r="B224">
         <v>378416000</v>
       </c>
-      <c r="C223">
+      <c r="C224">
         <v>4174977000</v>
       </c>
-      <c r="D223" t="s">
-        <v>389</v>
-      </c>
-      <c r="E223">
+      <c r="D224" t="s">
+        <v>391</v>
+      </c>
+      <c r="E224">
         <v>4174977</v>
       </c>
-      <c r="F223" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="I223" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B224">
+      <c r="F224" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="I224" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B225">
         <v>4175485000</v>
       </c>
-      <c r="C224">
+      <c r="C225">
         <v>4175485000</v>
       </c>
-      <c r="D224" t="s">
-        <v>502</v>
-      </c>
-      <c r="E224">
+      <c r="D225" t="s">
+        <v>504</v>
+      </c>
+      <c r="E225">
         <v>4175485</v>
       </c>
-      <c r="F224" s="1" t="s">
+      <c r="F225" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A225">
+    <row r="226" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A226">
         <v>4180790000</v>
       </c>
-      <c r="B225">
+      <c r="B226">
         <v>4180790000</v>
       </c>
-      <c r="C225">
+      <c r="C226">
         <v>4180790000</v>
-      </c>
-      <c r="D225" t="s">
-        <v>390</v>
-      </c>
-      <c r="E225">
-        <v>4180790</v>
-      </c>
-      <c r="F225" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="226" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A226">
-        <v>4181343000</v>
-      </c>
-      <c r="B226">
-        <v>4181343000</v>
-      </c>
-      <c r="C226">
-        <v>4181343000</v>
       </c>
       <c r="D226" t="s">
         <v>392</v>
       </c>
       <c r="E226">
-        <v>4181343</v>
+        <v>4180790</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>4181351000</v>
+        <v>4181343000</v>
       </c>
       <c r="B227">
-        <v>4181351000</v>
+        <v>4181343000</v>
       </c>
       <c r="C227">
-        <v>4181351000</v>
+        <v>4181343000</v>
       </c>
       <c r="D227" t="s">
         <v>394</v>
       </c>
       <c r="E227">
-        <v>4181351</v>
+        <v>4181343</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>4182210000</v>
+        <v>4181351000</v>
       </c>
       <c r="B228">
-        <v>4182210000</v>
+        <v>4181351000</v>
       </c>
       <c r="C228">
-        <v>4182210000</v>
+        <v>4181351000</v>
       </c>
       <c r="D228" t="s">
         <v>396</v>
       </c>
       <c r="E228">
-        <v>4182210</v>
+        <v>4181351</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>4182711000</v>
+        <v>4182210000</v>
       </c>
       <c r="B229">
-        <v>4137275000</v>
+        <v>4182210000</v>
       </c>
       <c r="C229">
-        <v>4182711000</v>
+        <v>4182210000</v>
       </c>
       <c r="D229" t="s">
         <v>398</v>
       </c>
       <c r="E229">
-        <v>4182711</v>
+        <v>4182210</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="H229" t="s">
+    </row>
+    <row r="230" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>4182711000</v>
+      </c>
+      <c r="B230">
+        <v>4137275000</v>
+      </c>
+      <c r="C230">
+        <v>4182711000</v>
+      </c>
+      <c r="D230" t="s">
         <v>400</v>
       </c>
-      <c r="I229" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="230" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A230">
+      <c r="E230">
+        <v>4182711</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="H230" t="s">
+        <v>402</v>
+      </c>
+      <c r="I230" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A231">
         <v>4185711000</v>
       </c>
-      <c r="B230">
+      <c r="B231">
         <v>4094294000</v>
       </c>
-      <c r="C230">
+      <c r="C231">
         <v>4185711000</v>
       </c>
-      <c r="D230" t="s">
-        <v>401</v>
-      </c>
-      <c r="E230">
+      <c r="D231" t="s">
+        <v>403</v>
+      </c>
+      <c r="E231">
         <v>4185711</v>
       </c>
-      <c r="F230" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="I230" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="231" spans="1:9" ht="270" x14ac:dyDescent="0.25">
-      <c r="A231">
+      <c r="F231" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="I231" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+      <c r="A232">
         <v>4185932000</v>
       </c>
-      <c r="B231">
+      <c r="B232">
         <v>4185932000</v>
       </c>
-      <c r="C231">
+      <c r="C232">
         <v>4185932000</v>
       </c>
-      <c r="D231" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="E231">
+      <c r="D232" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="E232">
         <v>4185932</v>
       </c>
-      <c r="F231" s="1" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A232">
-        <v>4189294000</v>
-      </c>
-      <c r="B232">
-        <v>4189294000</v>
-      </c>
-      <c r="C232">
-        <v>4189294000</v>
-      </c>
-      <c r="D232" t="s">
-        <v>560</v>
-      </c>
-      <c r="E232">
-        <v>4189294</v>
+      <c r="F232" s="1" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233">
+        <v>4189294000</v>
+      </c>
+      <c r="B233">
+        <v>4189294000</v>
+      </c>
+      <c r="C233">
+        <v>4189294000</v>
+      </c>
+      <c r="D233" t="s">
+        <v>562</v>
+      </c>
+      <c r="E233">
+        <v>4189294</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A234">
         <v>4190307000</v>
       </c>
-      <c r="B233">
+      <c r="B234">
         <v>4190307000</v>
       </c>
-      <c r="C233">
+      <c r="C234">
         <v>4190307000</v>
       </c>
-      <c r="D233" t="s">
-        <v>402</v>
-      </c>
-      <c r="E233">
+      <c r="D234" t="s">
+        <v>404</v>
+      </c>
+      <c r="E234">
         <v>4190307</v>
       </c>
-      <c r="F233" s="1" t="s">
+      <c r="F234" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A234">
+    <row r="235" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A235">
         <v>4195694000</v>
       </c>
-      <c r="B234">
+      <c r="B235">
         <v>4195694000</v>
       </c>
-      <c r="C234">
+      <c r="C235">
         <v>4195694000</v>
       </c>
-      <c r="D234" t="s">
-        <v>403</v>
-      </c>
-      <c r="E234">
+      <c r="D235" t="s">
+        <v>405</v>
+      </c>
+      <c r="E235">
         <v>4195694</v>
       </c>
-      <c r="F234" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="H234" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="235" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A235">
+      <c r="F235" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H235" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A236">
         <v>4201096000</v>
       </c>
-      <c r="B235">
+      <c r="B236">
         <v>4190307000</v>
       </c>
-      <c r="C235">
+      <c r="C236">
         <v>4201096000</v>
-      </c>
-      <c r="D235" t="s">
-        <v>406</v>
-      </c>
-      <c r="E235">
-        <v>4201096</v>
-      </c>
-      <c r="F235" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="I235" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="236" spans="1:9" ht="240" x14ac:dyDescent="0.25">
-      <c r="A236">
-        <v>4212540000</v>
-      </c>
-      <c r="B236">
-        <v>4212540000</v>
-      </c>
-      <c r="C236">
-        <v>4212540000</v>
       </c>
       <c r="D236" t="s">
         <v>408</v>
       </c>
       <c r="E236">
-        <v>4212540</v>
+        <v>4201096</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="237" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="I236" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>4223659000</v>
+        <v>4212540000</v>
       </c>
       <c r="B237">
-        <v>4094294000</v>
+        <v>4212540000</v>
       </c>
       <c r="C237">
-        <v>4223659000</v>
+        <v>4212540000</v>
       </c>
       <c r="D237" t="s">
         <v>410</v>
       </c>
       <c r="E237">
+        <v>4212540</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>4223659000</v>
+      </c>
+      <c r="B238">
+        <v>4094294000</v>
+      </c>
+      <c r="C238">
+        <v>4223659000</v>
+      </c>
+      <c r="D238" t="s">
+        <v>412</v>
+      </c>
+      <c r="E238">
         <v>4223659</v>
       </c>
-      <c r="F237" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="I237" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A238">
+      <c r="F238" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="I238" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A239">
         <v>4236484000</v>
       </c>
-      <c r="B238">
+      <c r="B239">
         <v>4236484000</v>
       </c>
-      <c r="C238">
+      <c r="C239">
         <v>4236484000</v>
-      </c>
-      <c r="D238" t="s">
-        <v>411</v>
-      </c>
-      <c r="E238">
-        <v>4236484</v>
-      </c>
-      <c r="F238" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A239">
-        <v>4245975000</v>
-      </c>
-      <c r="B239">
-        <v>4245975000</v>
-      </c>
-      <c r="C239">
-        <v>4245975000</v>
       </c>
       <c r="D239" t="s">
         <v>413</v>
       </c>
       <c r="E239">
-        <v>4245975</v>
+        <v>4236484</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>4246127000</v>
+        <v>4245975000</v>
       </c>
       <c r="B240">
-        <v>4246127000</v>
+        <v>4245975000</v>
       </c>
       <c r="C240">
-        <v>4246127000</v>
+        <v>4245975000</v>
       </c>
       <c r="D240" t="s">
         <v>415</v>
       </c>
       <c r="E240">
-        <v>4246127</v>
+        <v>4245975</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="H240" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="241" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>4253901000</v>
+        <v>4246127000</v>
       </c>
       <c r="B241">
-        <v>73553000</v>
+        <v>4246127000</v>
       </c>
       <c r="C241">
-        <v>4253901000</v>
+        <v>4246127000</v>
       </c>
       <c r="D241" t="s">
         <v>417</v>
       </c>
       <c r="E241">
-        <v>4253901</v>
+        <v>4246127</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I241" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="242" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="H241" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>4256228000</v>
+        <v>4253901000</v>
       </c>
       <c r="B242">
-        <v>4256228000</v>
+        <v>73553000</v>
       </c>
       <c r="C242">
-        <v>4256228000</v>
+        <v>4253901000</v>
       </c>
       <c r="D242" t="s">
         <v>419</v>
       </c>
       <c r="E242">
-        <v>4256228</v>
+        <v>4253901</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="H242" t="s">
+      <c r="I242" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>4256228000</v>
+      </c>
+      <c r="B243">
+        <v>4256228000</v>
+      </c>
+      <c r="C243">
+        <v>4256228000</v>
+      </c>
+      <c r="D243" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="243" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A243">
-        <v>4260535000</v>
-      </c>
-      <c r="B243">
-        <v>4043371000</v>
-      </c>
-      <c r="C243">
-        <v>4260535000</v>
-      </c>
-      <c r="D243" t="s">
+      <c r="E243">
+        <v>4256228</v>
+      </c>
+      <c r="F243" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="E243">
-        <v>4260535</v>
-      </c>
-      <c r="F243" s="1" t="s">
-        <v>479</v>
       </c>
       <c r="H243" t="s">
         <v>423</v>
       </c>
-      <c r="I243" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="244" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="244" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A244">
-        <v>4266367000</v>
+        <v>4260535000</v>
       </c>
       <c r="B244">
-        <v>4266367000</v>
+        <v>4043371000</v>
       </c>
       <c r="C244">
-        <v>4266367000</v>
+        <v>4260535000</v>
       </c>
       <c r="D244" t="s">
         <v>424</v>
       </c>
       <c r="E244">
-        <v>4266367</v>
+        <v>4260535</v>
       </c>
       <c r="F244" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="H244" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="245" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I244" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>4272240000</v>
+        <v>4266367000</v>
       </c>
       <c r="B245">
-        <v>4094294000</v>
+        <v>4266367000</v>
       </c>
       <c r="C245">
-        <v>4272240000</v>
+        <v>4266367000</v>
       </c>
       <c r="D245" t="s">
         <v>426</v>
       </c>
       <c r="E245">
+        <v>4266367</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>4272240000</v>
+      </c>
+      <c r="B246">
+        <v>4094294000</v>
+      </c>
+      <c r="C246">
+        <v>4272240000</v>
+      </c>
+      <c r="D246" t="s">
+        <v>428</v>
+      </c>
+      <c r="E246">
         <v>4272240</v>
       </c>
-      <c r="F245" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="I245" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="246" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A246">
+      <c r="F246" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="I246" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A247">
         <v>4273391000</v>
       </c>
-      <c r="B246">
+      <c r="B247">
         <v>4273391000</v>
       </c>
-      <c r="C246">
+      <c r="C247">
         <v>4273391000</v>
-      </c>
-      <c r="D246" t="s">
-        <v>427</v>
-      </c>
-      <c r="E246">
-        <v>4273391</v>
-      </c>
-      <c r="F246" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="247" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A247">
-        <v>4281232000</v>
-      </c>
-      <c r="B247">
-        <v>4212540000</v>
-      </c>
-      <c r="C247">
-        <v>4281232000</v>
       </c>
       <c r="D247" t="s">
         <v>429</v>
       </c>
       <c r="E247">
-        <v>4281232</v>
+        <v>4273391</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="I247" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="248" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A248">
+        <v>4281232000</v>
+      </c>
+      <c r="B248">
+        <v>4212540000</v>
+      </c>
+      <c r="C248">
+        <v>4281232000</v>
+      </c>
+      <c r="D248" t="s">
+        <v>431</v>
+      </c>
+      <c r="E248">
+        <v>4281232</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="I248" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A249">
         <v>4284492000</v>
       </c>
-      <c r="B248">
+      <c r="B249">
         <v>140168000</v>
       </c>
-      <c r="C248">
+      <c r="C249">
         <v>4284492000</v>
       </c>
-      <c r="D248" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="E248">
+      <c r="D249" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E249">
         <v>4284492</v>
       </c>
-      <c r="F248" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="I248" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="249" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A249">
+      <c r="F249" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="I249" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A250">
         <v>4285717000</v>
       </c>
-      <c r="B249">
+      <c r="B250">
         <v>4285717000</v>
       </c>
-      <c r="C249">
+      <c r="C250">
         <v>4285717000</v>
-      </c>
-      <c r="D249" t="s">
-        <v>432</v>
-      </c>
-      <c r="E249">
-        <v>4285717</v>
-      </c>
-      <c r="F249" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="250" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A250">
-        <v>4286201000</v>
-      </c>
-      <c r="B250">
-        <v>4286201000</v>
-      </c>
-      <c r="C250">
-        <v>4286201000</v>
       </c>
       <c r="D250" t="s">
         <v>434</v>
       </c>
       <c r="E250">
-        <v>4286201</v>
+        <v>4285717</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>435</v>
@@ -8033,240 +8039,237 @@
     </row>
     <row r="251" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>4290976000</v>
+        <v>4286201000</v>
       </c>
       <c r="B251">
-        <v>4137275000</v>
+        <v>4286201000</v>
       </c>
       <c r="C251">
-        <v>4290976000</v>
+        <v>4286201000</v>
       </c>
       <c r="D251" t="s">
         <v>436</v>
       </c>
       <c r="E251">
-        <v>4290976</v>
+        <v>4286201</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="I251" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="252" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>4299535000</v>
+        <v>4290976000</v>
       </c>
       <c r="B252">
-        <v>4299535000</v>
+        <v>4137275000</v>
       </c>
       <c r="C252">
-        <v>4299535000</v>
+        <v>4290976000</v>
       </c>
       <c r="D252" t="s">
         <v>438</v>
       </c>
       <c r="E252">
-        <v>4299535</v>
+        <v>4290976</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I252" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A253">
-        <v>4306655000</v>
+        <v>4299535000</v>
       </c>
       <c r="B253">
-        <v>4306655000</v>
+        <v>4299535000</v>
       </c>
       <c r="C253">
-        <v>4306655000</v>
+        <v>4299535000</v>
       </c>
       <c r="D253" t="s">
         <v>440</v>
       </c>
       <c r="E253">
-        <v>4306655</v>
+        <v>4299535</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="254" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254">
-        <v>4311499000</v>
+        <v>4306655000</v>
       </c>
       <c r="B254">
-        <v>4311499000</v>
+        <v>4306655000</v>
       </c>
       <c r="C254">
-        <v>4311499000</v>
+        <v>4306655000</v>
       </c>
       <c r="D254" t="s">
         <v>442</v>
       </c>
       <c r="E254">
-        <v>4311499</v>
+        <v>4306655</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="H254" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="255" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="255" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A255">
-        <v>4318985000</v>
+        <v>4311499000</v>
       </c>
       <c r="B255">
-        <v>378416000</v>
+        <v>4311499000</v>
       </c>
       <c r="C255">
-        <v>4318985000</v>
+        <v>4311499000</v>
       </c>
       <c r="D255" t="s">
         <v>444</v>
       </c>
       <c r="E255">
+        <v>4311499</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H255" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>4318985000</v>
+      </c>
+      <c r="B256">
+        <v>378416000</v>
+      </c>
+      <c r="C256">
+        <v>4318985000</v>
+      </c>
+      <c r="D256" t="s">
+        <v>446</v>
+      </c>
+      <c r="E256">
         <v>4318985</v>
       </c>
-      <c r="F255" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="I255" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="256" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A256">
+      <c r="F256" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="I256" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A257">
         <v>4322024000</v>
       </c>
-      <c r="B256">
+      <c r="B257">
         <v>4322024000</v>
       </c>
-      <c r="C256">
+      <c r="C257">
         <v>4322024000</v>
       </c>
-      <c r="D256" t="s">
-        <v>445</v>
-      </c>
-      <c r="E256">
+      <c r="D257" t="s">
+        <v>447</v>
+      </c>
+      <c r="E257">
         <v>4322024</v>
       </c>
-      <c r="F256" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="H256" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="257" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A257">
-        <v>4344489000</v>
-      </c>
-      <c r="B257">
-        <v>4137275000</v>
-      </c>
-      <c r="C257">
-        <v>4344489000</v>
-      </c>
-      <c r="D257" t="s">
+      <c r="F257" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E257">
-        <v>4344489</v>
-      </c>
-      <c r="F257" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="I257" t="s">
-        <v>22</v>
+      <c r="H257" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="258" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A258">
+        <v>4344489000</v>
+      </c>
+      <c r="B258">
+        <v>4137275000</v>
+      </c>
+      <c r="C258">
+        <v>4344489000</v>
+      </c>
+      <c r="D258" t="s">
+        <v>450</v>
+      </c>
+      <c r="E258">
+        <v>4344489</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="I258" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A259">
         <v>36712702000</v>
       </c>
-      <c r="B258">
+      <c r="B259">
         <v>36712702000</v>
       </c>
-      <c r="C258">
+      <c r="C259">
         <v>36712702000</v>
-      </c>
-      <c r="D258" t="s">
-        <v>449</v>
-      </c>
-      <c r="E258">
-        <v>36712702</v>
-      </c>
-      <c r="F258" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="259" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A259">
-        <v>37311061000</v>
-      </c>
-      <c r="B259">
-        <v>37311061000</v>
-      </c>
-      <c r="C259">
-        <v>37311061000</v>
       </c>
       <c r="D259" t="s">
         <v>451</v>
       </c>
       <c r="E259">
-        <v>37311061</v>
+        <v>36712702</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A260">
-        <v>40479589000</v>
+        <v>37311061000</v>
       </c>
       <c r="B260">
-        <v>321319000</v>
+        <v>37311061000</v>
       </c>
       <c r="C260">
-        <v>40479589000</v>
+        <v>37311061000</v>
       </c>
       <c r="D260" t="s">
         <v>453</v>
       </c>
       <c r="E260">
-        <v>40479589</v>
+        <v>37311061</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="I260" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="261" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="261" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A261">
-        <v>40481901000</v>
+        <v>40479589000</v>
       </c>
       <c r="B261">
-        <v>432571000</v>
+        <v>321319000</v>
       </c>
       <c r="C261">
-        <v>40481901000</v>
+        <v>40479589000</v>
       </c>
       <c r="D261" t="s">
         <v>455</v>
       </c>
       <c r="E261">
-        <v>40481901</v>
+        <v>40479589</v>
       </c>
       <c r="F261" s="1" t="s">
-        <v>513</v>
+        <v>456</v>
       </c>
       <c r="I261" t="s">
         <v>22</v>
@@ -8274,213 +8277,236 @@
     </row>
     <row r="262" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A262">
+        <v>40481901000</v>
+      </c>
+      <c r="B262">
+        <v>432571000</v>
+      </c>
+      <c r="C262">
+        <v>40481901000</v>
+      </c>
+      <c r="D262" t="s">
+        <v>457</v>
+      </c>
+      <c r="E262">
+        <v>40481901</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="I262" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A263">
         <v>40481902000</v>
       </c>
-      <c r="B262">
+      <c r="B263">
         <v>40481902000</v>
       </c>
-      <c r="C262">
+      <c r="C263">
         <v>40481902000</v>
       </c>
-      <c r="D262" t="s">
-        <v>456</v>
-      </c>
-      <c r="E262">
+      <c r="D263" t="s">
+        <v>458</v>
+      </c>
+      <c r="E263">
         <v>40481902</v>
       </c>
-      <c r="F262" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="H262" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="263" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A263">
-        <v>40490918000</v>
-      </c>
-      <c r="B263">
-        <v>432571000</v>
-      </c>
-      <c r="C263">
-        <v>40490918000</v>
-      </c>
-      <c r="D263" t="s">
+      <c r="F263" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="E263">
-        <v>40490918</v>
-      </c>
-      <c r="F263" s="1" t="s">
-        <v>514</v>
-      </c>
       <c r="H263" t="s">
-        <v>24</v>
-      </c>
-      <c r="I263" t="s">
-        <v>22</v>
+        <v>460</v>
       </c>
     </row>
     <row r="264" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A264">
+        <v>40490918000</v>
+      </c>
+      <c r="B264">
+        <v>432571000</v>
+      </c>
+      <c r="C264">
+        <v>40490918000</v>
+      </c>
+      <c r="D264" t="s">
+        <v>461</v>
+      </c>
+      <c r="E264">
+        <v>40490918</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="H264" t="s">
+        <v>24</v>
+      </c>
+      <c r="I264" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A265">
         <v>42535714000</v>
       </c>
-      <c r="B264">
+      <c r="B265">
         <v>4137275000</v>
       </c>
-      <c r="C264">
+      <c r="C265">
         <v>42535714000</v>
-      </c>
-      <c r="D264" t="s">
-        <v>460</v>
-      </c>
-      <c r="E264">
-        <v>42535714</v>
-      </c>
-      <c r="F264" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="I264" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="265" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A265">
-        <v>43021132000</v>
-      </c>
-      <c r="B265">
-        <v>43021132000</v>
-      </c>
-      <c r="C265">
-        <v>43021132000</v>
       </c>
       <c r="D265" t="s">
         <v>462</v>
       </c>
       <c r="E265">
-        <v>43021132</v>
+        <v>42535714</v>
       </c>
       <c r="F265" s="1" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I265" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A266">
+        <v>43021132000</v>
+      </c>
+      <c r="B266">
+        <v>43021132000</v>
+      </c>
+      <c r="C266">
+        <v>43021132000</v>
+      </c>
+      <c r="D266" t="s">
+        <v>464</v>
+      </c>
+      <c r="E266">
+        <v>43021132</v>
+      </c>
+      <c r="F266" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A267">
         <v>43021226000</v>
       </c>
-      <c r="B266">
+      <c r="B267">
         <v>43021226000</v>
       </c>
-      <c r="C266">
+      <c r="C267">
         <v>43021226000</v>
       </c>
-      <c r="D266" t="s">
-        <v>550</v>
-      </c>
-      <c r="E266">
+      <c r="D267" t="s">
+        <v>552</v>
+      </c>
+      <c r="E267">
         <v>43021226</v>
       </c>
-      <c r="F266" s="1" t="s">
+      <c r="F267" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="H266" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="267" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A267">
+      <c r="H267" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A268">
         <v>43530714000</v>
       </c>
-      <c r="B267">
+      <c r="B268">
         <v>4094294000</v>
       </c>
-      <c r="C267">
+      <c r="C268">
         <v>43530714000</v>
       </c>
-      <c r="D267" t="s">
-        <v>464</v>
-      </c>
-      <c r="E267">
+      <c r="D268" t="s">
+        <v>466</v>
+      </c>
+      <c r="E268">
         <v>43530714</v>
       </c>
-      <c r="F267" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="I267" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="268" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A268">
+      <c r="F268" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="I268" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A269">
         <v>44784217000</v>
       </c>
-      <c r="B268">
+      <c r="B269">
         <v>44784217000</v>
       </c>
-      <c r="C268">
+      <c r="C269">
         <v>44784217000</v>
       </c>
-      <c r="D268" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="E268">
+      <c r="D269" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="E269">
         <v>44784217</v>
       </c>
-      <c r="F268" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="H268" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="269" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A269">
+      <c r="F269" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="H269" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A270">
         <v>45763653000</v>
       </c>
-      <c r="B269">
+      <c r="B270">
         <v>45763653000</v>
       </c>
-      <c r="C269">
+      <c r="C270">
         <v>45763653000</v>
-      </c>
-      <c r="D269" t="s">
-        <v>468</v>
-      </c>
-      <c r="E269">
-        <v>45763653</v>
-      </c>
-      <c r="F269" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="H269" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="270" spans="1:9" ht="270" x14ac:dyDescent="0.25">
-      <c r="A270">
-        <v>46271022000</v>
-      </c>
-      <c r="B270">
-        <v>4030518000</v>
-      </c>
-      <c r="C270">
-        <v>46271022000</v>
       </c>
       <c r="D270" t="s">
         <v>470</v>
       </c>
       <c r="E270">
-        <v>46271022</v>
+        <v>45763653</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="I270" t="s">
+      <c r="H270" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>46271022000</v>
+      </c>
+      <c r="B271">
+        <v>4030518000</v>
+      </c>
+      <c r="C271">
+        <v>46271022000</v>
+      </c>
+      <c r="D271" t="s">
+        <v>472</v>
+      </c>
+      <c r="E271">
+        <v>46271022</v>
+      </c>
+      <c r="F271" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="I271" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I270">
+  <autoFilter ref="A1:I271">
     <sortState ref="A2:I271">
       <sortCondition ref="C1:C271"/>
     </sortState>

</xml_diff>